<commit_message>
Update api  get orders
</commit_message>
<xml_diff>
--- a/Database ToCoShop.xlsx
+++ b/Database ToCoShop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="115">
   <si>
     <t>No.</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Foreign Key</t>
   </si>
   <si>
-    <t>EmployeeId</t>
-  </si>
-  <si>
     <t>Reference Employees (Id)</t>
   </si>
   <si>
@@ -353,6 +350,15 @@
   </si>
   <si>
     <t>CompanyPhoneNumber</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>NameUser</t>
+  </si>
+  <si>
+    <t>firstName + lastName from Employees(Id)</t>
   </si>
 </sst>
 </file>
@@ -947,24 +953,6 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -990,8 +978,26 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1299,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I130"/>
+  <dimension ref="A2:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1320,28 +1326,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
     </row>
     <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
+      <c r="A3" s="120"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
     </row>
     <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -1482,28 +1488,28 @@
       <c r="I9" s="24"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="109" t="s">
+      <c r="A12" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="109"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
+      <c r="A13" s="117"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
@@ -1680,28 +1686,28 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="111" t="s">
+      <c r="A24" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
+      <c r="B24" s="121"/>
+      <c r="C24" s="121"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="121"/>
     </row>
     <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="111"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="111"/>
-      <c r="I25" s="111"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
+      <c r="I25" s="121"/>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -1813,19 +1819,19 @@
         <v>36</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="119">
+      <c r="A31" s="113">
         <v>5</v>
       </c>
       <c r="B31" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16"/>
@@ -1835,7 +1841,7 @@
       <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="120"/>
+      <c r="A32" s="114"/>
       <c r="B32" s="10" t="s">
         <v>26</v>
       </c>
@@ -1849,12 +1855,12 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="120"/>
+      <c r="A33" s="114"/>
       <c r="B33" s="10" t="s">
         <v>25</v>
       </c>
@@ -1870,14 +1876,14 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="120"/>
+      <c r="A34" s="114"/>
       <c r="B34" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>14</v>
@@ -1892,9 +1898,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="120"/>
+      <c r="A35" s="114"/>
       <c r="B35" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>14</v>
@@ -1909,26 +1915,26 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A36" s="120"/>
+      <c r="A36" s="114"/>
       <c r="B36" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="31"/>
+      <c r="E36" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="117"/>
-      <c r="G36" s="117"/>
-      <c r="H36" s="117"/>
-      <c r="I36" s="118"/>
+      <c r="F36" s="111"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="111"/>
+      <c r="I36" s="112"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="120"/>
+      <c r="A37" s="114"/>
       <c r="B37" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>14</v>
@@ -1943,9 +1949,9 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="120"/>
+      <c r="A38" s="114"/>
       <c r="B38" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>14</v>
@@ -1960,9 +1966,9 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="121"/>
+      <c r="A39" s="115"/>
       <c r="B39" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>14</v>
@@ -1977,14 +1983,14 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="119">
+      <c r="A40" s="113">
         <v>6</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="16"/>
@@ -1994,9 +2000,9 @@
       <c r="I40" s="14"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="120"/>
+      <c r="A41" s="114"/>
       <c r="B41" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>10</v>
@@ -2008,14 +2014,14 @@
       </c>
       <c r="G41" s="10"/>
       <c r="H41" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="120"/>
+      <c r="A42" s="114"/>
       <c r="B42" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>14</v>
@@ -2030,9 +2036,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="120"/>
+      <c r="A43" s="114"/>
       <c r="B43" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>14</v>
@@ -2047,7 +2053,7 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="120"/>
+      <c r="A44" s="114"/>
       <c r="B44" s="10" t="s">
         <v>26</v>
       </c>
@@ -2061,31 +2067,31 @@
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
       <c r="H44" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A45" s="120"/>
+      <c r="A45" s="114"/>
       <c r="B45" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="31"/>
-      <c r="E45" s="116" t="s">
-        <v>80</v>
-      </c>
-      <c r="F45" s="117"/>
-      <c r="G45" s="117"/>
-      <c r="H45" s="117"/>
-      <c r="I45" s="118"/>
+      <c r="E45" s="110" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="111"/>
+      <c r="G45" s="111"/>
+      <c r="H45" s="111"/>
+      <c r="I45" s="112"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="120"/>
+      <c r="A46" s="114"/>
       <c r="B46" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>14</v>
@@ -2100,9 +2106,9 @@
       <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="120"/>
+      <c r="A47" s="114"/>
       <c r="B47" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>14</v>
@@ -2117,9 +2123,9 @@
       <c r="I47" s="10"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="120"/>
+      <c r="A48" s="114"/>
       <c r="B48" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>14</v>
@@ -2134,9 +2140,9 @@
       <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="120"/>
+      <c r="A49" s="114"/>
       <c r="B49" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>14</v>
@@ -2153,9 +2159,9 @@
       <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="121"/>
+      <c r="A50" s="115"/>
       <c r="B50" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>14</v>
@@ -2172,14 +2178,14 @@
       <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="119">
+      <c r="A51" s="113">
         <v>7</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="16"/>
@@ -2189,9 +2195,9 @@
       <c r="I51" s="14"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="120"/>
+      <c r="A52" s="114"/>
       <c r="B52" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>14</v>
@@ -2201,31 +2207,31 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A53" s="114"/>
+      <c r="B53" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I52" s="10"/>
-    </row>
-    <row r="53" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A53" s="120"/>
-      <c r="B53" s="29" t="s">
+      <c r="C53" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="31"/>
+      <c r="E53" s="110" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53" s="111"/>
+      <c r="G53" s="111"/>
+      <c r="H53" s="111"/>
+      <c r="I53" s="112"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="114"/>
+      <c r="B54" s="32" t="s">
         <v>62</v>
-      </c>
-      <c r="C53" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D53" s="31"/>
-      <c r="E53" s="116" t="s">
-        <v>70</v>
-      </c>
-      <c r="F53" s="117"/>
-      <c r="G53" s="117"/>
-      <c r="H53" s="117"/>
-      <c r="I53" s="118"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="120"/>
-      <c r="B54" s="32" t="s">
-        <v>63</v>
       </c>
       <c r="C54" s="33" t="s">
         <v>14</v>
@@ -2235,14 +2241,14 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I54" s="10"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="120"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="33" t="s">
         <v>14</v>
@@ -2257,9 +2263,9 @@
       <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="120"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="33" t="s">
         <v>31</v>
@@ -2269,16 +2275,16 @@
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="121"/>
+      <c r="A57" s="115"/>
       <c r="B57" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="33" t="s">
         <v>14</v>
@@ -2290,19 +2296,19 @@
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
       <c r="H57" s="104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I57" s="10"/>
     </row>
     <row r="58" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="122">
+      <c r="A58" s="118">
         <v>8</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
@@ -2312,9 +2318,9 @@
       <c r="I58" s="14"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="122"/>
+      <c r="A59" s="118"/>
       <c r="B59" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>10</v>
@@ -2326,17 +2332,17 @@
       </c>
       <c r="G59" s="10"/>
       <c r="H59" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I59" s="10"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="118"/>
+      <c r="B60" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I59" s="10"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="122"/>
-      <c r="B60" s="10" t="s">
+      <c r="C60" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13"/>
@@ -2346,12 +2352,12 @@
       <c r="I60" s="10"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="122"/>
+      <c r="A61" s="118"/>
       <c r="B61" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
@@ -2361,12 +2367,12 @@
       <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="122"/>
+      <c r="A62" s="118"/>
       <c r="B62" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
@@ -2376,14 +2382,14 @@
       <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="119">
+      <c r="A63" s="113">
         <v>9</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63" s="16"/>
@@ -2393,9 +2399,9 @@
       <c r="I63" s="14"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="120"/>
+      <c r="A64" s="114"/>
       <c r="B64" s="10" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>10</v>
@@ -2407,155 +2413,152 @@
       </c>
       <c r="G64" s="10"/>
       <c r="H64" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="121"/>
+      <c r="A65" s="114"/>
       <c r="B65" s="10" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="12">
+      <c r="D65" s="12"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="115"/>
+      <c r="B66" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="12">
         <v>500</v>
       </c>
-      <c r="E65" s="13"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
-      <c r="I65" s="10"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="109" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="109"/>
-      <c r="C68" s="109"/>
-      <c r="D68" s="109"/>
-      <c r="E68" s="109"/>
-      <c r="F68" s="109"/>
-      <c r="G68" s="109"/>
-      <c r="H68" s="109"/>
-      <c r="I68" s="109"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="110"/>
-      <c r="B69" s="110"/>
-      <c r="C69" s="110"/>
-      <c r="D69" s="110"/>
-      <c r="E69" s="110"/>
-      <c r="F69" s="110"/>
-      <c r="G69" s="110"/>
-      <c r="H69" s="110"/>
-      <c r="I69" s="110"/>
+      <c r="A69" s="116" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="116"/>
+      <c r="C69" s="116"/>
+      <c r="D69" s="116"/>
+      <c r="E69" s="116"/>
+      <c r="F69" s="116"/>
+      <c r="G69" s="116"/>
+      <c r="H69" s="116"/>
+      <c r="I69" s="116"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="45" t="s">
+      <c r="A70" s="117"/>
+      <c r="B70" s="117"/>
+      <c r="C70" s="117"/>
+      <c r="D70" s="117"/>
+      <c r="E70" s="117"/>
+      <c r="F70" s="117"/>
+      <c r="G70" s="117"/>
+      <c r="H70" s="117"/>
+      <c r="I70" s="117"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="45" t="s">
+      <c r="B71" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C70" s="45" t="s">
+      <c r="C71" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="45" t="s">
+      <c r="D71" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="45" t="s">
+      <c r="E71" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F70" s="45" t="s">
+      <c r="F71" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="45" t="s">
+      <c r="G71" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="45" t="s">
+      <c r="H71" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I70" s="45" t="s">
+      <c r="I71" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="46">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="46">
         <v>1</v>
       </c>
-      <c r="B71" s="46" t="s">
+      <c r="B72" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="47" t="s">
+      <c r="C72" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="48"/>
-      <c r="E71" s="49"/>
-      <c r="F71" s="46" t="s">
+      <c r="D72" s="48"/>
+      <c r="E72" s="49"/>
+      <c r="F72" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G71" s="46"/>
-      <c r="H71" s="46" t="s">
+      <c r="G72" s="46"/>
+      <c r="H72" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I71" s="46"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="50">
-        <f>A71+1</f>
-        <v>2</v>
-      </c>
-      <c r="B72" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C72" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="53">
-        <v>50</v>
-      </c>
-      <c r="E72" s="54"/>
-      <c r="F72" s="55"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="I72" s="55"/>
+      <c r="I72" s="46"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="50">
         <f>A72+1</f>
-        <v>3</v>
-      </c>
-      <c r="B73" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="D73" s="53"/>
+        <v>2</v>
+      </c>
+      <c r="B73" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="53">
+        <v>50</v>
+      </c>
       <c r="E73" s="54"/>
       <c r="F73" s="55"/>
       <c r="G73" s="55"/>
-      <c r="H73" s="50"/>
+      <c r="H73" s="50" t="s">
+        <v>15</v>
+      </c>
       <c r="I73" s="55"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="105">
-        <f t="shared" ref="A74:A77" si="2">A73+1</f>
-        <v>4</v>
-      </c>
-      <c r="B74" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="C74" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="53">
-        <v>50</v>
-      </c>
+      <c r="A74" s="50">
+        <f>A73+1</f>
+        <v>3</v>
+      </c>
+      <c r="B74" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="C74" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="53"/>
       <c r="E74" s="54"/>
       <c r="F74" s="55"/>
       <c r="G74" s="55"/>
@@ -2563,12 +2566,12 @@
       <c r="I74" s="55"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="50">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B75" s="106" t="s">
-        <v>111</v>
+      <c r="A75" s="105">
+        <f t="shared" ref="A75:A78" si="2">A74+1</f>
+        <v>4</v>
+      </c>
+      <c r="B75" s="51" t="s">
+        <v>109</v>
       </c>
       <c r="C75" s="52" t="s">
         <v>14</v>
@@ -2576,157 +2579,155 @@
       <c r="D75" s="53">
         <v>50</v>
       </c>
-      <c r="E75" s="56"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="50"/>
+      <c r="E75" s="54"/>
+      <c r="F75" s="55"/>
+      <c r="G75" s="55"/>
       <c r="H75" s="50"/>
-      <c r="I75" s="50"/>
+      <c r="I75" s="55"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="50">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B76" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C76" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="59">
+        <v>5</v>
+      </c>
+      <c r="B76" s="106" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="53">
         <v>50</v>
       </c>
-      <c r="E76" s="60"/>
-      <c r="F76" s="61"/>
-      <c r="G76" s="61"/>
-      <c r="H76" s="61"/>
-      <c r="I76" s="61"/>
+      <c r="E76" s="56"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
+      <c r="H76" s="50"/>
+      <c r="I76" s="50"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="50">
         <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B77" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="59">
+        <v>50</v>
+      </c>
+      <c r="E77" s="60"/>
+      <c r="F77" s="61"/>
+      <c r="G77" s="61"/>
+      <c r="H77" s="61"/>
+      <c r="I77" s="61"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="50">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B77" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="C77" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="63">
+      <c r="B78" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="63">
         <v>200</v>
       </c>
-      <c r="E77" s="56" t="s">
+      <c r="E78" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="F77" s="50"/>
-      <c r="G77" s="50"/>
-      <c r="H77" s="50"/>
-      <c r="I77" s="50"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="107" t="s">
-        <v>71</v>
-      </c>
-      <c r="B81" s="107"/>
-      <c r="C81" s="107"/>
-      <c r="D81" s="107"/>
-      <c r="E81" s="107"/>
-      <c r="F81" s="107"/>
-      <c r="G81" s="107"/>
-      <c r="H81" s="107"/>
-      <c r="I81" s="107"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="50"/>
+      <c r="H78" s="50"/>
+      <c r="I78" s="50"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="112"/>
-      <c r="B82" s="112"/>
-      <c r="C82" s="112"/>
-      <c r="D82" s="112"/>
-      <c r="E82" s="112"/>
-      <c r="F82" s="112"/>
-      <c r="G82" s="112"/>
-      <c r="H82" s="112"/>
-      <c r="I82" s="112"/>
+      <c r="A82" s="119" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" s="119"/>
+      <c r="C82" s="119"/>
+      <c r="D82" s="119"/>
+      <c r="E82" s="119"/>
+      <c r="F82" s="119"/>
+      <c r="G82" s="119"/>
+      <c r="H82" s="119"/>
+      <c r="I82" s="119"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="39" t="s">
+      <c r="A83" s="122"/>
+      <c r="B83" s="122"/>
+      <c r="C83" s="122"/>
+      <c r="D83" s="122"/>
+      <c r="E83" s="122"/>
+      <c r="F83" s="122"/>
+      <c r="G83" s="122"/>
+      <c r="H83" s="122"/>
+      <c r="I83" s="122"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B83" s="39" t="s">
+      <c r="B84" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C83" s="39" t="s">
+      <c r="C84" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D83" s="39" t="s">
+      <c r="D84" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E83" s="39" t="s">
+      <c r="E84" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F83" s="39" t="s">
+      <c r="F84" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G83" s="39" t="s">
+      <c r="G84" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H83" s="39" t="s">
+      <c r="H84" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I83" s="39" t="s">
+      <c r="I84" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="40">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="40">
         <v>1</v>
       </c>
-      <c r="B84" s="40" t="s">
+      <c r="B85" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="41" t="s">
+      <c r="C85" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D84" s="42"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="40" t="s">
+      <c r="D85" s="42"/>
+      <c r="E85" s="43"/>
+      <c r="F85" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G84" s="40"/>
-      <c r="H84" s="40" t="s">
+      <c r="G85" s="40"/>
+      <c r="H85" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I84" s="44"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="36">
-        <f>A84+1</f>
-        <v>2</v>
-      </c>
-      <c r="B85" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C85" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D85" s="37">
-        <v>50</v>
-      </c>
-      <c r="E85" s="38"/>
-      <c r="F85" s="36"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="I85" s="36"/>
+      <c r="I85" s="44"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="36">
-        <f t="shared" ref="A86:A88" si="3">A85+1</f>
-        <v>3</v>
+        <f>A85+1</f>
+        <v>2</v>
       </c>
       <c r="B86" s="36" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C86" s="35" t="s">
         <v>14</v>
@@ -2737,321 +2738,324 @@
       <c r="E86" s="38"/>
       <c r="F86" s="36"/>
       <c r="G86" s="36"/>
-      <c r="H86" s="36"/>
+      <c r="H86" s="68" t="s">
+        <v>73</v>
+      </c>
       <c r="I86" s="36"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="36">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="B87" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C87" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D87" s="28">
+        <f t="shared" ref="A87:A89" si="3">A86+1</f>
+        <v>3</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="37">
         <v>50</v>
       </c>
-      <c r="E87" s="8"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H87" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="I87" s="24"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="36"/>
+      <c r="I87" s="36"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="36">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="B88" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C88" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="D88" s="37"/>
-      <c r="E88" s="38"/>
-      <c r="F88" s="36"/>
+        <v>4</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="28">
+        <v>50</v>
+      </c>
+      <c r="E88" s="8"/>
+      <c r="F88" s="24"/>
       <c r="G88" s="24" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H88" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="I88" s="36"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="67"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="107" t="s">
-        <v>81</v>
-      </c>
-      <c r="B94" s="107"/>
-      <c r="C94" s="107"/>
-      <c r="D94" s="107"/>
-      <c r="E94" s="107"/>
-      <c r="F94" s="107"/>
-      <c r="G94" s="107"/>
-      <c r="H94" s="107"/>
-      <c r="I94" s="107"/>
+      <c r="I88" s="24"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="36">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B89" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D89" s="37"/>
+      <c r="E89" s="38"/>
+      <c r="F89" s="36"/>
+      <c r="G89" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H89" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I89" s="36"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="67"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="112"/>
-      <c r="B95" s="112"/>
-      <c r="C95" s="112"/>
-      <c r="D95" s="112"/>
-      <c r="E95" s="112"/>
-      <c r="F95" s="112"/>
-      <c r="G95" s="112"/>
-      <c r="H95" s="112"/>
-      <c r="I95" s="112"/>
+      <c r="A95" s="119" t="s">
+        <v>80</v>
+      </c>
+      <c r="B95" s="119"/>
+      <c r="C95" s="119"/>
+      <c r="D95" s="119"/>
+      <c r="E95" s="119"/>
+      <c r="F95" s="119"/>
+      <c r="G95" s="119"/>
+      <c r="H95" s="119"/>
+      <c r="I95" s="119"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="39" t="s">
+      <c r="A96" s="122"/>
+      <c r="B96" s="122"/>
+      <c r="C96" s="122"/>
+      <c r="D96" s="122"/>
+      <c r="E96" s="122"/>
+      <c r="F96" s="122"/>
+      <c r="G96" s="122"/>
+      <c r="H96" s="122"/>
+      <c r="I96" s="122"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B96" s="39" t="s">
+      <c r="B97" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C96" s="39" t="s">
+      <c r="C97" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D96" s="39" t="s">
+      <c r="D97" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E96" s="39" t="s">
+      <c r="E97" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F96" s="39" t="s">
+      <c r="F97" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G96" s="39" t="s">
+      <c r="G97" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H96" s="39" t="s">
+      <c r="H97" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I96" s="39" t="s">
+      <c r="I97" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="40">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="40">
         <v>1</v>
       </c>
-      <c r="B97" s="40" t="s">
+      <c r="B98" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="41" t="s">
+      <c r="C98" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D97" s="42"/>
-      <c r="E97" s="43"/>
-      <c r="F97" s="40" t="s">
+      <c r="D98" s="42"/>
+      <c r="E98" s="43"/>
+      <c r="F98" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G97" s="40"/>
-      <c r="H97" s="40" t="s">
+      <c r="G98" s="40"/>
+      <c r="H98" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I97" s="44"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="36">
-        <f>A97+1</f>
-        <v>2</v>
-      </c>
-      <c r="B98" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C98" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D98" s="37">
-        <v>50</v>
-      </c>
-      <c r="E98" s="38"/>
-      <c r="F98" s="36"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="68"/>
-      <c r="I98" s="36"/>
+      <c r="I98" s="44"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="36">
-        <f t="shared" ref="A99:A101" si="4">A98+1</f>
-        <v>3</v>
+        <f>A98+1</f>
+        <v>2</v>
       </c>
       <c r="B99" s="36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C99" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D99" s="37">
-        <v>500</v>
-      </c>
-      <c r="E99" s="38" t="s">
-        <v>17</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E99" s="38"/>
       <c r="F99" s="36"/>
       <c r="G99" s="36"/>
-      <c r="H99" s="36"/>
+      <c r="H99" s="68"/>
       <c r="I99" s="36"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="36">
+        <f t="shared" ref="A100:A102" si="4">A99+1</f>
+        <v>3</v>
+      </c>
+      <c r="B100" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" s="37">
+        <v>500</v>
+      </c>
+      <c r="E100" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F100" s="36"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="36"/>
+      <c r="I100" s="36"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="36">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B100" s="27" t="s">
+      <c r="B101" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C100" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D100" s="28" t="s">
+      <c r="C101" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E100" s="8"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="24"/>
-      <c r="H100" s="24"/>
-      <c r="I100" s="24"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="69">
+      <c r="E101" s="8"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+      <c r="I101" s="24"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="69">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B101" s="69" t="s">
+      <c r="B102" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C102" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="C101" s="70" t="s">
+      <c r="D102" s="71"/>
+      <c r="E102" s="72"/>
+      <c r="F102" s="69"/>
+      <c r="G102" s="73"/>
+      <c r="H102" s="73"/>
+      <c r="I102" s="69"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="74">
+        <v>6</v>
+      </c>
+      <c r="B103" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" s="74"/>
+      <c r="E103" s="74"/>
+      <c r="F103" s="74"/>
+      <c r="G103" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="H103" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="I103" s="74"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="D101" s="71"/>
-      <c r="E101" s="72"/>
-      <c r="F101" s="69"/>
-      <c r="G101" s="73"/>
-      <c r="H101" s="73"/>
-      <c r="I101" s="69"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="74">
+      <c r="B107" s="108"/>
+      <c r="C107" s="108"/>
+      <c r="D107" s="108"/>
+      <c r="E107" s="108"/>
+      <c r="F107" s="77"/>
+      <c r="G107" s="77"/>
+      <c r="H107" s="77"/>
+      <c r="I107" s="77"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="E108" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="F108" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="G108" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="C102" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" s="74"/>
-      <c r="E102" s="74"/>
-      <c r="F102" s="74"/>
-      <c r="G102" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="H102" s="75" t="s">
-        <v>79</v>
-      </c>
-      <c r="I102" s="74"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="B106" s="114"/>
-      <c r="C106" s="114"/>
-      <c r="D106" s="114"/>
-      <c r="E106" s="114"/>
-      <c r="F106" s="77"/>
-      <c r="G106" s="77"/>
-      <c r="H106" s="77"/>
-      <c r="I106" s="77"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B107" s="78" t="s">
+      <c r="H108" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="I108" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="79">
         <v>1</v>
       </c>
-      <c r="C107" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D107" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="E107" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="F107" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="G107" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="H107" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="I107" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="79">
-        <v>1</v>
-      </c>
-      <c r="B108" s="79" t="s">
+      <c r="B109" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C108" s="80" t="s">
+      <c r="C109" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="81">
+      <c r="D109" s="81">
         <v>50</v>
       </c>
-      <c r="E108" s="82"/>
-      <c r="F108" s="79" t="s">
+      <c r="E109" s="82"/>
+      <c r="F109" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G108" s="79"/>
-      <c r="H108" s="79"/>
-      <c r="I108" s="79"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="83">
-        <v>2</v>
-      </c>
-      <c r="B109" s="83" t="s">
-        <v>59</v>
-      </c>
-      <c r="C109" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D109" s="85">
-        <v>50</v>
-      </c>
-      <c r="E109" s="86"/>
-      <c r="F109" s="83"/>
-      <c r="G109" s="83"/>
-      <c r="H109" s="83"/>
-      <c r="I109" s="83"/>
+      <c r="G109" s="79"/>
+      <c r="H109" s="79"/>
+      <c r="I109" s="79"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B110" s="83" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C110" s="84" t="s">
         <v>14</v>
@@ -3067,10 +3071,10 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B111" s="83" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C111" s="84" t="s">
         <v>14</v>
@@ -3078,9 +3082,7 @@
       <c r="D111" s="85">
         <v>50</v>
       </c>
-      <c r="E111" s="86" t="s">
-        <v>17</v>
-      </c>
+      <c r="E111" s="86"/>
       <c r="F111" s="83"/>
       <c r="G111" s="83"/>
       <c r="H111" s="83"/>
@@ -3088,18 +3090,20 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B112" s="83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C112" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D112" s="85">
-        <v>500</v>
-      </c>
-      <c r="E112" s="86"/>
+        <v>50</v>
+      </c>
+      <c r="E112" s="86" t="s">
+        <v>17</v>
+      </c>
       <c r="F112" s="83"/>
       <c r="G112" s="83"/>
       <c r="H112" s="83"/>
@@ -3107,54 +3111,62 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B113" s="83" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C113" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D113" s="85">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E113" s="86"/>
       <c r="F113" s="83"/>
       <c r="G113" s="83"/>
-      <c r="H113" s="83" t="s">
+      <c r="H113" s="83"/>
+      <c r="I113" s="83"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" s="83">
+        <v>6</v>
+      </c>
+      <c r="B114" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C114" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" s="85">
+        <v>50</v>
+      </c>
+      <c r="E114" s="86"/>
+      <c r="F114" s="83"/>
+      <c r="G114" s="83"/>
+      <c r="H114" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="I113" s="83"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="98">
+      <c r="I114" s="83"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" s="98">
         <v>7</v>
       </c>
-      <c r="B114" s="98" t="s">
-        <v>88</v>
-      </c>
-      <c r="C114" s="99" t="s">
+      <c r="B115" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="C115" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="D114" s="100"/>
-      <c r="E114" s="101" t="s">
+      <c r="D115" s="100"/>
+      <c r="E115" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F114" s="98"/>
-      <c r="G114" s="98"/>
-      <c r="H114" s="98"/>
-      <c r="I114" s="98"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="94"/>
-      <c r="B115" s="94"/>
-      <c r="C115" s="95"/>
-      <c r="D115" s="96"/>
-      <c r="E115" s="97"/>
-      <c r="F115" s="94"/>
-      <c r="G115" s="94"/>
-      <c r="H115" s="94"/>
-      <c r="I115" s="94"/>
+      <c r="F115" s="98"/>
+      <c r="G115" s="98"/>
+      <c r="H115" s="98"/>
+      <c r="I115" s="98"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="94"/>
@@ -3168,128 +3180,118 @@
       <c r="I116" s="94"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="102"/>
-      <c r="B117" s="102"/>
-      <c r="C117" s="102"/>
-      <c r="D117" s="102"/>
-      <c r="E117" s="102"/>
-      <c r="F117" s="102"/>
-      <c r="G117" s="102"/>
-      <c r="H117" s="102"/>
-      <c r="I117" s="102"/>
+      <c r="A117" s="94"/>
+      <c r="B117" s="94"/>
+      <c r="C117" s="95"/>
+      <c r="D117" s="96"/>
+      <c r="E117" s="97"/>
+      <c r="F117" s="94"/>
+      <c r="G117" s="94"/>
+      <c r="H117" s="94"/>
+      <c r="I117" s="94"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="115" t="s">
-        <v>89</v>
-      </c>
-      <c r="B118" s="114"/>
-      <c r="C118" s="114"/>
-      <c r="D118" s="114"/>
-      <c r="E118" s="114"/>
-      <c r="F118" s="87"/>
-      <c r="G118" s="87"/>
-      <c r="H118" s="87"/>
-      <c r="I118" s="87"/>
+      <c r="A118" s="102"/>
+      <c r="B118" s="102"/>
+      <c r="C118" s="102"/>
+      <c r="D118" s="102"/>
+      <c r="E118" s="102"/>
+      <c r="F118" s="102"/>
+      <c r="G118" s="102"/>
+      <c r="H118" s="102"/>
+      <c r="I118" s="102"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="88" t="s">
+      <c r="A119" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="B119" s="108"/>
+      <c r="C119" s="108"/>
+      <c r="D119" s="108"/>
+      <c r="E119" s="108"/>
+      <c r="F119" s="87"/>
+      <c r="G119" s="87"/>
+      <c r="H119" s="87"/>
+      <c r="I119" s="87"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B119" s="88" t="s">
+      <c r="B120" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C119" s="88" t="s">
+      <c r="C120" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D119" s="88" t="s">
+      <c r="D120" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E119" s="88" t="s">
+      <c r="E120" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F119" s="88" t="s">
+      <c r="F120" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G119" s="88" t="s">
+      <c r="G120" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H119" s="88" t="s">
+      <c r="H120" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I119" s="88" t="s">
+      <c r="I120" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="1">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
         <v>1</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C120" s="89" t="s">
+      <c r="C121" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="90"/>
-      <c r="E120" s="91"/>
-      <c r="F120" s="1" t="s">
+      <c r="D121" s="90"/>
+      <c r="E121" s="91"/>
+      <c r="F121" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1" t="s">
+      <c r="G121" s="1"/>
+      <c r="H121" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I120" s="1"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="2">
-        <v>2</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D121" s="92">
-        <v>50</v>
-      </c>
-      <c r="E121" s="93"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="6"/>
-      <c r="H121" s="6"/>
-      <c r="I121" s="6"/>
+      <c r="I121" s="1"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D122" s="4"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2">
-        <v>0</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I122" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D122" s="92">
+        <v>50</v>
+      </c>
+      <c r="E122" s="93"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="5"/>
@@ -3298,19 +3300,19 @@
         <v>0</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I123" s="2"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="5"/>
@@ -3318,36 +3320,36 @@
       <c r="G124" s="2">
         <v>0</v>
       </c>
-      <c r="H124" s="2"/>
+      <c r="H124" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="I124" s="2"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="5"/>
-      <c r="F125" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G125" s="2"/>
-      <c r="H125" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2">
+        <v>0</v>
+      </c>
+      <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>10</v>
@@ -3359,102 +3361,123 @@
       </c>
       <c r="G126" s="2"/>
       <c r="H126" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
+        <v>7</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127" s="4"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G127" s="2"/>
+      <c r="H127" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I127" s="2"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
         <v>8</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C127" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D127" s="4" t="s">
+      <c r="C128" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E127" s="5"/>
-      <c r="F127" s="6"/>
-      <c r="G127" s="2"/>
-      <c r="H127" s="6"/>
-      <c r="I127" s="2"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="103">
-        <v>9</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D128" s="4"/>
       <c r="E128" s="5"/>
       <c r="F128" s="6"/>
       <c r="G128" s="2"/>
       <c r="H128" s="6"/>
-      <c r="I128" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="I128" s="2"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="103">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="5"/>
       <c r="F129" s="6"/>
       <c r="G129" s="2"/>
       <c r="H129" s="6"/>
-      <c r="I129" s="2"/>
+      <c r="I129" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" s="2">
-        <v>11</v>
+      <c r="A130" s="103">
+        <v>10</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="5"/>
       <c r="F130" s="6"/>
       <c r="G130" s="2"/>
       <c r="H130" s="6"/>
-      <c r="I130" s="2" t="s">
-        <v>100</v>
+      <c r="I130" s="2"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>11</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D131" s="4"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A106:E106"/>
-    <mergeCell ref="A118:E118"/>
+    <mergeCell ref="A2:I3"/>
+    <mergeCell ref="A12:I13"/>
+    <mergeCell ref="A24:I25"/>
+    <mergeCell ref="A82:I83"/>
+    <mergeCell ref="A95:I96"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A119:E119"/>
     <mergeCell ref="E36:I36"/>
     <mergeCell ref="A40:A50"/>
     <mergeCell ref="E45:I45"/>
-    <mergeCell ref="A68:I69"/>
+    <mergeCell ref="A69:I70"/>
     <mergeCell ref="E53:I53"/>
     <mergeCell ref="A58:A62"/>
     <mergeCell ref="A51:A57"/>
-    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A63:A66"/>
     <mergeCell ref="A31:A39"/>
-    <mergeCell ref="A2:I3"/>
-    <mergeCell ref="A12:I13"/>
-    <mergeCell ref="A24:I25"/>
-    <mergeCell ref="A81:I82"/>
-    <mergeCell ref="A94:I95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update backend and frontendAdmin
</commit_message>
<xml_diff>
--- a/Database ToCoShop.xlsx
+++ b/Database ToCoShop.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="Orders" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="124">
   <si>
     <t>No.</t>
   </si>
@@ -115,12 +116,6 @@
     <t>GETDATE()</t>
   </si>
   <si>
-    <t>Check ShippedDate &gt;= CreatedDate</t>
-  </si>
-  <si>
-    <t>ShippedDate</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -359,6 +354,39 @@
   </si>
   <si>
     <t>firstName + lastName from Employees(Id)</t>
+  </si>
+  <si>
+    <t>Mã đơn hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày đặt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng tiền </t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Ngày gửi</t>
+  </si>
+  <si>
+    <t>Ngày nhận</t>
+  </si>
+  <si>
+    <t>SendingDate</t>
+  </si>
+  <si>
+    <t>Check SendingDate &gt;= CreatedDate</t>
+  </si>
+  <si>
+    <t>Check ShippedDate &gt;= SendingDate</t>
+  </si>
+  <si>
+    <t>ReceivedDate</t>
+  </si>
+  <si>
+    <t>Check CreatedDate&lt;= today</t>
   </si>
 </sst>
 </file>
@@ -953,6 +981,24 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -978,26 +1024,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1305,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I131"/>
+  <dimension ref="A2:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1326,28 +1354,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
     </row>
     <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="120"/>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
     </row>
     <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -1488,28 +1516,28 @@
       <c r="I9" s="24"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="117"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="117"/>
+      <c r="A13" s="110"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
@@ -1686,28 +1714,28 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="121"/>
-      <c r="C24" s="121"/>
-      <c r="D24" s="121"/>
-      <c r="E24" s="121"/>
-      <c r="F24" s="121"/>
-      <c r="G24" s="121"/>
-      <c r="H24" s="121"/>
-      <c r="I24" s="121"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
     </row>
     <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="121"/>
-      <c r="B25" s="121"/>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="121"/>
-      <c r="G25" s="121"/>
-      <c r="H25" s="121"/>
-      <c r="I25" s="121"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="111"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="111"/>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -1777,7 +1805,7 @@
         <v>32</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="I28" s="10"/>
     </row>
@@ -1786,7 +1814,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>31</v>
@@ -1798,71 +1826,73 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
+        <v>3</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
         <v>4</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="113">
+      <c r="B31" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="119">
         <v>5</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="114"/>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="120"/>
+      <c r="B33" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="12">
-        <v>50</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="114"/>
-      <c r="B33" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>14</v>
@@ -1870,20 +1900,18 @@
       <c r="D33" s="12">
         <v>50</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="E33" s="13"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="114"/>
+      <c r="A34" s="120"/>
       <c r="B34" s="10" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>14</v>
@@ -1891,16 +1919,20 @@
       <c r="D34" s="12">
         <v>50</v>
       </c>
-      <c r="E34" s="13"/>
+      <c r="E34" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
+      <c r="H34" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="114"/>
+      <c r="A35" s="120"/>
       <c r="B35" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>14</v>
@@ -1914,44 +1946,44 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A36" s="114"/>
-      <c r="B36" s="29" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="120"/>
+      <c r="B36" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="12">
+        <v>50</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A37" s="120"/>
+      <c r="B37" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="110" t="s">
-        <v>66</v>
-      </c>
-      <c r="F36" s="111"/>
-      <c r="G36" s="111"/>
-      <c r="H36" s="111"/>
-      <c r="I36" s="112"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="114"/>
-      <c r="B37" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="34">
-        <v>50</v>
-      </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
+      <c r="C37" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="31"/>
+      <c r="E37" s="116" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="117"/>
+      <c r="G37" s="117"/>
+      <c r="H37" s="117"/>
+      <c r="I37" s="118"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="114"/>
+      <c r="A38" s="120"/>
       <c r="B38" s="32" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>14</v>
@@ -1966,15 +1998,15 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="115"/>
+      <c r="A39" s="120"/>
       <c r="B39" s="32" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="34" t="s">
-        <v>23</v>
+      <c r="D39" s="34">
+        <v>50</v>
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="10"/>
@@ -1982,63 +2014,63 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="113">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="121"/>
+      <c r="B40" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+    </row>
+    <row r="41" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="119">
         <v>6</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="114"/>
-      <c r="B41" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="11" t="s">
+      <c r="B41" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="120"/>
+      <c r="B42" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="I41" s="10"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="114"/>
-      <c r="B42" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="12">
-        <v>50</v>
-      </c>
+      <c r="D42" s="12"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="10"/>
+      <c r="F42" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
+      <c r="H42" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="114"/>
+      <c r="A43" s="120"/>
       <c r="B43" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>14</v>
@@ -2053,9 +2085,9 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="114"/>
+      <c r="A44" s="120"/>
       <c r="B44" s="10" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>14</v>
@@ -2066,49 +2098,49 @@
       <c r="E44" s="13"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="14" t="s">
-        <v>106</v>
-      </c>
+      <c r="H44" s="10"/>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A45" s="114"/>
-      <c r="B45" s="29" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="120"/>
+      <c r="B45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="12">
+        <v>50</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I45" s="10"/>
+    </row>
+    <row r="46" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A46" s="120"/>
+      <c r="B46" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="110" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="112"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="114"/>
-      <c r="B46" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="34">
-        <v>50</v>
-      </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
+      <c r="C46" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="31"/>
+      <c r="E46" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="117"/>
+      <c r="G46" s="117"/>
+      <c r="H46" s="117"/>
+      <c r="I46" s="118"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="114"/>
+      <c r="A47" s="120"/>
       <c r="B47" s="32" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>14</v>
@@ -2123,15 +2155,15 @@
       <c r="I47" s="10"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="114"/>
+      <c r="A48" s="120"/>
       <c r="B48" s="32" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="34" t="s">
-        <v>23</v>
+      <c r="D48" s="34">
+        <v>50</v>
       </c>
       <c r="E48" s="13"/>
       <c r="F48" s="10"/>
@@ -2140,28 +2172,26 @@
       <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="114"/>
-      <c r="B49" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="12">
-        <v>200</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A49" s="120"/>
+      <c r="B49" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="13"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="115"/>
+      <c r="A50" s="120"/>
       <c r="B50" s="10" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>14</v>
@@ -2177,202 +2207,206 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="113">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="121"/>
+      <c r="B51" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="12">
+        <v>200</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="119">
         <v>7</v>
       </c>
-      <c r="B51" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="9" t="s">
+      <c r="B52" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="15"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="114"/>
-      <c r="B52" s="10" t="s">
+      <c r="C52" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="120"/>
+      <c r="B53" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A54" s="120"/>
+      <c r="B54" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10" t="s">
+      <c r="C54" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" s="31"/>
+      <c r="E54" s="116" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="117"/>
+      <c r="G54" s="117"/>
+      <c r="H54" s="117"/>
+      <c r="I54" s="118"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="120"/>
+      <c r="B55" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="I52" s="10"/>
-    </row>
-    <row r="53" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A53" s="114"/>
-      <c r="B53" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" s="31"/>
-      <c r="E53" s="110" t="s">
-        <v>69</v>
-      </c>
-      <c r="F53" s="111"/>
-      <c r="G53" s="111"/>
-      <c r="H53" s="111"/>
-      <c r="I53" s="112"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="114"/>
-      <c r="B54" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="34"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I54" s="10"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="114"/>
-      <c r="B55" s="32" t="s">
-        <v>102</v>
-      </c>
       <c r="C55" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="34">
-        <v>50</v>
-      </c>
+      <c r="D55" s="34"/>
       <c r="E55" s="13"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
+      <c r="H55" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="114"/>
+      <c r="A56" s="120"/>
       <c r="B56" s="32" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="34"/>
+        <v>14</v>
+      </c>
+      <c r="D56" s="34">
+        <v>50</v>
+      </c>
       <c r="E56" s="13"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
-      <c r="H56" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I56" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="115"/>
+      <c r="A57" s="120"/>
       <c r="B57" s="32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="34">
-        <v>3</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D57" s="34"/>
       <c r="E57" s="13"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="104" t="s">
-        <v>105</v>
-      </c>
-      <c r="I57" s="10"/>
-    </row>
-    <row r="58" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="118">
+      <c r="H57" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="121"/>
+      <c r="B58" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="34">
+        <v>3</v>
+      </c>
+      <c r="E58" s="13"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="104" t="s">
+        <v>103</v>
+      </c>
+      <c r="I58" s="10"/>
+    </row>
+    <row r="59" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="122">
         <v>8</v>
       </c>
-      <c r="B58" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="118"/>
-      <c r="B59" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C59" s="11" t="s">
+      <c r="B59" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="122"/>
+      <c r="B60" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G59" s="10"/>
-      <c r="H59" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I59" s="10"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="118"/>
-      <c r="B60" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13"/>
-      <c r="F60" s="10"/>
+      <c r="F60" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
+      <c r="H60" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="I60" s="10"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="118"/>
+      <c r="A61" s="122"/>
       <c r="B61" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="13"/>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="118"/>
+      <c r="A62" s="122"/>
       <c r="B62" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
@@ -2382,203 +2416,198 @@
       <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="113">
+      <c r="A63" s="122"/>
+      <c r="B63" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="119">
         <v>9</v>
       </c>
-      <c r="B63" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D63" s="15"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="114"/>
-      <c r="B64" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="11" t="s">
+      <c r="B64" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="120"/>
+      <c r="B65" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="D64" s="12"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G64" s="10"/>
-      <c r="H64" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I64" s="10"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="114"/>
-      <c r="B65" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>14</v>
       </c>
       <c r="D65" s="12"/>
       <c r="E65" s="13"/>
-      <c r="F65" s="14"/>
+      <c r="F65" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G65" s="10"/>
       <c r="H65" s="14" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="115"/>
+      <c r="A66" s="120"/>
       <c r="B66" s="10" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="12">
+      <c r="D66" s="12"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I66" s="10"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="121"/>
+      <c r="B67" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="12">
         <v>500</v>
       </c>
-      <c r="E66" s="13"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="B69" s="116"/>
-      <c r="C69" s="116"/>
-      <c r="D69" s="116"/>
-      <c r="E69" s="116"/>
-      <c r="F69" s="116"/>
-      <c r="G69" s="116"/>
-      <c r="H69" s="116"/>
-      <c r="I69" s="116"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="117"/>
-      <c r="B70" s="117"/>
-      <c r="C70" s="117"/>
-      <c r="D70" s="117"/>
-      <c r="E70" s="117"/>
-      <c r="F70" s="117"/>
-      <c r="G70" s="117"/>
-      <c r="H70" s="117"/>
-      <c r="I70" s="117"/>
+      <c r="A70" s="109" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="109"/>
+      <c r="C70" s="109"/>
+      <c r="D70" s="109"/>
+      <c r="E70" s="109"/>
+      <c r="F70" s="109"/>
+      <c r="G70" s="109"/>
+      <c r="H70" s="109"/>
+      <c r="I70" s="109"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="45" t="s">
+      <c r="A71" s="110"/>
+      <c r="B71" s="110"/>
+      <c r="C71" s="110"/>
+      <c r="D71" s="110"/>
+      <c r="E71" s="110"/>
+      <c r="F71" s="110"/>
+      <c r="G71" s="110"/>
+      <c r="H71" s="110"/>
+      <c r="I71" s="110"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="45" t="s">
+      <c r="B72" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="45" t="s">
+      <c r="C72" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D71" s="45" t="s">
+      <c r="D72" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E71" s="45" t="s">
+      <c r="E72" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F71" s="45" t="s">
+      <c r="F72" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G71" s="45" t="s">
+      <c r="G72" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H71" s="45" t="s">
+      <c r="H72" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I71" s="45" t="s">
+      <c r="I72" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="46">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="46">
         <v>1</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B73" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="47" t="s">
+      <c r="C73" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D72" s="48"/>
-      <c r="E72" s="49"/>
-      <c r="F72" s="46" t="s">
+      <c r="D73" s="48"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G72" s="46"/>
-      <c r="H72" s="46" t="s">
+      <c r="G73" s="46"/>
+      <c r="H73" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I72" s="46"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="50">
-        <f>A72+1</f>
-        <v>2</v>
-      </c>
-      <c r="B73" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="53">
-        <v>50</v>
-      </c>
-      <c r="E73" s="54"/>
-      <c r="F73" s="55"/>
-      <c r="G73" s="55"/>
-      <c r="H73" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="I73" s="55"/>
+      <c r="I73" s="46"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="50">
         <f>A73+1</f>
-        <v>3</v>
-      </c>
-      <c r="B74" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="C74" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" s="53"/>
+        <v>2</v>
+      </c>
+      <c r="B74" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="53">
+        <v>50</v>
+      </c>
       <c r="E74" s="54"/>
       <c r="F74" s="55"/>
       <c r="G74" s="55"/>
-      <c r="H74" s="50"/>
+      <c r="H74" s="50" t="s">
+        <v>15</v>
+      </c>
       <c r="I74" s="55"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="105">
-        <f t="shared" ref="A75:A78" si="2">A74+1</f>
-        <v>4</v>
-      </c>
-      <c r="B75" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="53">
-        <v>50</v>
-      </c>
+      <c r="A75" s="50">
+        <f>A74+1</f>
+        <v>3</v>
+      </c>
+      <c r="B75" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="53"/>
       <c r="E75" s="54"/>
       <c r="F75" s="55"/>
       <c r="G75" s="55"/>
@@ -2586,12 +2615,12 @@
       <c r="I75" s="55"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="50">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B76" s="106" t="s">
-        <v>110</v>
+      <c r="A76" s="105">
+        <f t="shared" ref="A76:A79" si="2">A75+1</f>
+        <v>4</v>
+      </c>
+      <c r="B76" s="51" t="s">
+        <v>107</v>
       </c>
       <c r="C76" s="52" t="s">
         <v>14</v>
@@ -2599,157 +2628,155 @@
       <c r="D76" s="53">
         <v>50</v>
       </c>
-      <c r="E76" s="56"/>
-      <c r="F76" s="50"/>
-      <c r="G76" s="50"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="55"/>
+      <c r="G76" s="55"/>
       <c r="H76" s="50"/>
-      <c r="I76" s="50"/>
+      <c r="I76" s="55"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="50">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B77" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="C77" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="59">
+        <v>5</v>
+      </c>
+      <c r="B77" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="C77" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="53">
         <v>50</v>
       </c>
-      <c r="E77" s="60"/>
-      <c r="F77" s="61"/>
-      <c r="G77" s="61"/>
-      <c r="H77" s="61"/>
-      <c r="I77" s="61"/>
+      <c r="E77" s="56"/>
+      <c r="F77" s="50"/>
+      <c r="G77" s="50"/>
+      <c r="H77" s="50"/>
+      <c r="I77" s="50"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="50">
         <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B78" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="59">
+        <v>50</v>
+      </c>
+      <c r="E78" s="60"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="61"/>
+      <c r="H78" s="61"/>
+      <c r="I78" s="61"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="50">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B78" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C78" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="63">
+      <c r="B79" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="63">
         <v>200</v>
       </c>
-      <c r="E78" s="56" t="s">
+      <c r="E79" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="F78" s="50"/>
-      <c r="G78" s="50"/>
-      <c r="H78" s="50"/>
-      <c r="I78" s="50"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="119" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" s="119"/>
-      <c r="C82" s="119"/>
-      <c r="D82" s="119"/>
-      <c r="E82" s="119"/>
-      <c r="F82" s="119"/>
-      <c r="G82" s="119"/>
-      <c r="H82" s="119"/>
-      <c r="I82" s="119"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="50"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="122"/>
-      <c r="B83" s="122"/>
-      <c r="C83" s="122"/>
-      <c r="D83" s="122"/>
-      <c r="E83" s="122"/>
-      <c r="F83" s="122"/>
-      <c r="G83" s="122"/>
-      <c r="H83" s="122"/>
-      <c r="I83" s="122"/>
+      <c r="A83" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="107"/>
+      <c r="C83" s="107"/>
+      <c r="D83" s="107"/>
+      <c r="E83" s="107"/>
+      <c r="F83" s="107"/>
+      <c r="G83" s="107"/>
+      <c r="H83" s="107"/>
+      <c r="I83" s="107"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="112"/>
+      <c r="B84" s="112"/>
+      <c r="C84" s="112"/>
+      <c r="D84" s="112"/>
+      <c r="E84" s="112"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="112"/>
+      <c r="H84" s="112"/>
+      <c r="I84" s="112"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="39" t="s">
+      <c r="B85" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C84" s="39" t="s">
+      <c r="C85" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D84" s="39" t="s">
+      <c r="D85" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E84" s="39" t="s">
+      <c r="E85" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F84" s="39" t="s">
+      <c r="F85" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G84" s="39" t="s">
+      <c r="G85" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H84" s="39" t="s">
+      <c r="H85" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I84" s="39" t="s">
+      <c r="I85" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="40">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="40">
         <v>1</v>
       </c>
-      <c r="B85" s="40" t="s">
+      <c r="B86" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="41" t="s">
+      <c r="C86" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D85" s="42"/>
-      <c r="E85" s="43"/>
-      <c r="F85" s="40" t="s">
+      <c r="D86" s="42"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G85" s="40"/>
-      <c r="H85" s="40" t="s">
+      <c r="G86" s="40"/>
+      <c r="H86" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I85" s="44"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="36">
-        <f>A85+1</f>
-        <v>2</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C86" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D86" s="37">
-        <v>50</v>
-      </c>
-      <c r="E86" s="38"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="I86" s="36"/>
+      <c r="I86" s="44"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="36">
-        <f t="shared" ref="A87:A89" si="3">A86+1</f>
-        <v>3</v>
+        <f>A86+1</f>
+        <v>2</v>
       </c>
       <c r="B87" s="36" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="C87" s="35" t="s">
         <v>14</v>
@@ -2760,321 +2787,324 @@
       <c r="E87" s="38"/>
       <c r="F87" s="36"/>
       <c r="G87" s="36"/>
-      <c r="H87" s="36"/>
+      <c r="H87" s="68" t="s">
+        <v>71</v>
+      </c>
       <c r="I87" s="36"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="36">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="B88" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C88" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" s="28">
+        <f t="shared" ref="A88:A90" si="3">A87+1</f>
+        <v>3</v>
+      </c>
+      <c r="B88" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C88" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="37">
         <v>50</v>
       </c>
-      <c r="E88" s="8"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="H88" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="I88" s="24"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="36"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="36"/>
+      <c r="I88" s="36"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="36">
         <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="28">
+        <v>50</v>
+      </c>
+      <c r="E89" s="8"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H89" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I89" s="24"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="36">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B89" s="36" t="s">
+      <c r="B90" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="37"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="36"/>
+      <c r="G90" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C89" s="35" t="s">
+      <c r="H90" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D89" s="37"/>
-      <c r="E89" s="38"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="H89" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I89" s="36"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="67"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="119" t="s">
-        <v>80</v>
-      </c>
-      <c r="B95" s="119"/>
-      <c r="C95" s="119"/>
-      <c r="D95" s="119"/>
-      <c r="E95" s="119"/>
-      <c r="F95" s="119"/>
-      <c r="G95" s="119"/>
-      <c r="H95" s="119"/>
-      <c r="I95" s="119"/>
+      <c r="I90" s="36"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="67"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="122"/>
-      <c r="B96" s="122"/>
-      <c r="C96" s="122"/>
-      <c r="D96" s="122"/>
-      <c r="E96" s="122"/>
-      <c r="F96" s="122"/>
-      <c r="G96" s="122"/>
-      <c r="H96" s="122"/>
-      <c r="I96" s="122"/>
+      <c r="A96" s="107" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" s="107"/>
+      <c r="C96" s="107"/>
+      <c r="D96" s="107"/>
+      <c r="E96" s="107"/>
+      <c r="F96" s="107"/>
+      <c r="G96" s="107"/>
+      <c r="H96" s="107"/>
+      <c r="I96" s="107"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="39" t="s">
+      <c r="A97" s="112"/>
+      <c r="B97" s="112"/>
+      <c r="C97" s="112"/>
+      <c r="D97" s="112"/>
+      <c r="E97" s="112"/>
+      <c r="F97" s="112"/>
+      <c r="G97" s="112"/>
+      <c r="H97" s="112"/>
+      <c r="I97" s="112"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B97" s="39" t="s">
+      <c r="B98" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C97" s="39" t="s">
+      <c r="C98" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D97" s="39" t="s">
+      <c r="D98" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E97" s="39" t="s">
+      <c r="E98" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F97" s="39" t="s">
+      <c r="F98" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G97" s="39" t="s">
+      <c r="G98" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H97" s="39" t="s">
+      <c r="H98" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I97" s="39" t="s">
+      <c r="I98" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="40">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="40">
         <v>1</v>
       </c>
-      <c r="B98" s="40" t="s">
+      <c r="B99" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="41" t="s">
+      <c r="C99" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D98" s="42"/>
-      <c r="E98" s="43"/>
-      <c r="F98" s="40" t="s">
+      <c r="D99" s="42"/>
+      <c r="E99" s="43"/>
+      <c r="F99" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G98" s="40"/>
-      <c r="H98" s="40" t="s">
+      <c r="G99" s="40"/>
+      <c r="H99" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I98" s="44"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="36">
-        <f>A98+1</f>
-        <v>2</v>
-      </c>
-      <c r="B99" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C99" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D99" s="37">
-        <v>50</v>
-      </c>
-      <c r="E99" s="38"/>
-      <c r="F99" s="36"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="68"/>
-      <c r="I99" s="36"/>
+      <c r="I99" s="44"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="36">
-        <f t="shared" ref="A100:A102" si="4">A99+1</f>
-        <v>3</v>
+        <f>A99+1</f>
+        <v>2</v>
       </c>
       <c r="B100" s="36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C100" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D100" s="37">
-        <v>500</v>
-      </c>
-      <c r="E100" s="38" t="s">
-        <v>17</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E100" s="38"/>
       <c r="F100" s="36"/>
       <c r="G100" s="36"/>
-      <c r="H100" s="36"/>
+      <c r="H100" s="68"/>
       <c r="I100" s="36"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="36">
+        <f t="shared" ref="A101:A103" si="4">A100+1</f>
+        <v>3</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C101" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="37">
+        <v>500</v>
+      </c>
+      <c r="E101" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F101" s="36"/>
+      <c r="G101" s="36"/>
+      <c r="H101" s="36"/>
+      <c r="I101" s="36"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="36">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B101" s="27" t="s">
+      <c r="B102" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C101" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D101" s="28" t="s">
+      <c r="C102" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E101" s="8"/>
-      <c r="F101" s="24"/>
-      <c r="G101" s="24"/>
-      <c r="H101" s="24"/>
-      <c r="I101" s="24"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="69">
+      <c r="E102" s="8"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="69">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B102" s="69" t="s">
+      <c r="B103" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="C103" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="D103" s="71"/>
+      <c r="E103" s="72"/>
+      <c r="F103" s="69"/>
+      <c r="G103" s="73"/>
+      <c r="H103" s="73"/>
+      <c r="I103" s="69"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="74">
+        <v>6</v>
+      </c>
+      <c r="B104" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="74"/>
+      <c r="G104" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="H104" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="I104" s="74"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="C102" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="D102" s="71"/>
-      <c r="E102" s="72"/>
-      <c r="F102" s="69"/>
-      <c r="G102" s="73"/>
-      <c r="H102" s="73"/>
-      <c r="I102" s="69"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="74">
+      <c r="B108" s="114"/>
+      <c r="C108" s="114"/>
+      <c r="D108" s="114"/>
+      <c r="E108" s="114"/>
+      <c r="F108" s="77"/>
+      <c r="G108" s="77"/>
+      <c r="H108" s="77"/>
+      <c r="I108" s="77"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="F109" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="G109" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B103" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="C103" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" s="74"/>
-      <c r="E103" s="74"/>
-      <c r="F103" s="74"/>
-      <c r="G103" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="H103" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="I103" s="74"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="107" t="s">
-        <v>85</v>
-      </c>
-      <c r="B107" s="108"/>
-      <c r="C107" s="108"/>
-      <c r="D107" s="108"/>
-      <c r="E107" s="108"/>
-      <c r="F107" s="77"/>
-      <c r="G107" s="77"/>
-      <c r="H107" s="77"/>
-      <c r="I107" s="77"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B108" s="78" t="s">
+      <c r="H109" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="I109" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="79">
         <v>1</v>
       </c>
-      <c r="C108" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D108" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="E108" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="F108" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="G108" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="H108" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="I108" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="79">
-        <v>1</v>
-      </c>
-      <c r="B109" s="79" t="s">
+      <c r="B110" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C109" s="80" t="s">
+      <c r="C110" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D109" s="81">
+      <c r="D110" s="81">
         <v>50</v>
       </c>
-      <c r="E109" s="82"/>
-      <c r="F109" s="79" t="s">
+      <c r="E110" s="82"/>
+      <c r="F110" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G109" s="79"/>
-      <c r="H109" s="79"/>
-      <c r="I109" s="79"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="83">
-        <v>2</v>
-      </c>
-      <c r="B110" s="83" t="s">
-        <v>58</v>
-      </c>
-      <c r="C110" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D110" s="85">
-        <v>50</v>
-      </c>
-      <c r="E110" s="86"/>
-      <c r="F110" s="83"/>
-      <c r="G110" s="83"/>
-      <c r="H110" s="83"/>
-      <c r="I110" s="83"/>
+      <c r="G110" s="79"/>
+      <c r="H110" s="79"/>
+      <c r="I110" s="79"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B111" s="83" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C111" s="84" t="s">
         <v>14</v>
@@ -3090,10 +3120,10 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B112" s="83" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="C112" s="84" t="s">
         <v>14</v>
@@ -3101,9 +3131,7 @@
       <c r="D112" s="85">
         <v>50</v>
       </c>
-      <c r="E112" s="86" t="s">
-        <v>17</v>
-      </c>
+      <c r="E112" s="86"/>
       <c r="F112" s="83"/>
       <c r="G112" s="83"/>
       <c r="H112" s="83"/>
@@ -3111,18 +3139,20 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B113" s="83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C113" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D113" s="85">
-        <v>500</v>
-      </c>
-      <c r="E113" s="86"/>
+        <v>50</v>
+      </c>
+      <c r="E113" s="86" t="s">
+        <v>17</v>
+      </c>
       <c r="F113" s="83"/>
       <c r="G113" s="83"/>
       <c r="H113" s="83"/>
@@ -3130,54 +3160,62 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B114" s="83" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C114" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D114" s="85">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E114" s="86"/>
       <c r="F114" s="83"/>
       <c r="G114" s="83"/>
-      <c r="H114" s="83" t="s">
+      <c r="H114" s="83"/>
+      <c r="I114" s="83"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" s="83">
+        <v>6</v>
+      </c>
+      <c r="B115" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C115" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="85">
+        <v>50</v>
+      </c>
+      <c r="E115" s="86"/>
+      <c r="F115" s="83"/>
+      <c r="G115" s="83"/>
+      <c r="H115" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="I114" s="83"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="98">
+      <c r="I115" s="83"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" s="98">
         <v>7</v>
       </c>
-      <c r="B115" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="C115" s="99" t="s">
+      <c r="B116" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="C116" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="D115" s="100"/>
-      <c r="E115" s="101" t="s">
+      <c r="D116" s="100"/>
+      <c r="E116" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F115" s="98"/>
-      <c r="G115" s="98"/>
-      <c r="H115" s="98"/>
-      <c r="I115" s="98"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="94"/>
-      <c r="B116" s="94"/>
-      <c r="C116" s="95"/>
-      <c r="D116" s="96"/>
-      <c r="E116" s="97"/>
-      <c r="F116" s="94"/>
-      <c r="G116" s="94"/>
-      <c r="H116" s="94"/>
-      <c r="I116" s="94"/>
+      <c r="F116" s="98"/>
+      <c r="G116" s="98"/>
+      <c r="H116" s="98"/>
+      <c r="I116" s="98"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="94"/>
@@ -3191,128 +3229,118 @@
       <c r="I117" s="94"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="102"/>
-      <c r="B118" s="102"/>
-      <c r="C118" s="102"/>
-      <c r="D118" s="102"/>
-      <c r="E118" s="102"/>
-      <c r="F118" s="102"/>
-      <c r="G118" s="102"/>
-      <c r="H118" s="102"/>
-      <c r="I118" s="102"/>
+      <c r="A118" s="94"/>
+      <c r="B118" s="94"/>
+      <c r="C118" s="95"/>
+      <c r="D118" s="96"/>
+      <c r="E118" s="97"/>
+      <c r="F118" s="94"/>
+      <c r="G118" s="94"/>
+      <c r="H118" s="94"/>
+      <c r="I118" s="94"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="109" t="s">
-        <v>88</v>
-      </c>
-      <c r="B119" s="108"/>
-      <c r="C119" s="108"/>
-      <c r="D119" s="108"/>
-      <c r="E119" s="108"/>
-      <c r="F119" s="87"/>
-      <c r="G119" s="87"/>
-      <c r="H119" s="87"/>
-      <c r="I119" s="87"/>
+      <c r="A119" s="102"/>
+      <c r="B119" s="102"/>
+      <c r="C119" s="102"/>
+      <c r="D119" s="102"/>
+      <c r="E119" s="102"/>
+      <c r="F119" s="102"/>
+      <c r="G119" s="102"/>
+      <c r="H119" s="102"/>
+      <c r="I119" s="102"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="88" t="s">
+      <c r="A120" s="115" t="s">
+        <v>86</v>
+      </c>
+      <c r="B120" s="114"/>
+      <c r="C120" s="114"/>
+      <c r="D120" s="114"/>
+      <c r="E120" s="114"/>
+      <c r="F120" s="87"/>
+      <c r="G120" s="87"/>
+      <c r="H120" s="87"/>
+      <c r="I120" s="87"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B120" s="88" t="s">
+      <c r="B121" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C120" s="88" t="s">
+      <c r="C121" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D120" s="88" t="s">
+      <c r="D121" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E120" s="88" t="s">
+      <c r="E121" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F120" s="88" t="s">
+      <c r="F121" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G120" s="88" t="s">
+      <c r="G121" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H120" s="88" t="s">
+      <c r="H121" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I120" s="88" t="s">
+      <c r="I121" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="1">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
         <v>1</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C121" s="89" t="s">
+      <c r="C122" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D121" s="90"/>
-      <c r="E121" s="91"/>
-      <c r="F121" s="1" t="s">
+      <c r="D122" s="90"/>
+      <c r="E122" s="91"/>
+      <c r="F122" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1" t="s">
+      <c r="G122" s="1"/>
+      <c r="H122" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I121" s="1"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="2">
-        <v>2</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D122" s="92">
-        <v>50</v>
-      </c>
-      <c r="E122" s="93"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="6"/>
-      <c r="H122" s="6"/>
-      <c r="I122" s="6"/>
+      <c r="I122" s="1"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D123" s="4"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="2"/>
-      <c r="G123" s="2">
-        <v>0</v>
-      </c>
-      <c r="H123" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I123" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D123" s="92">
+        <v>50</v>
+      </c>
+      <c r="E123" s="93"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="5"/>
@@ -3321,19 +3349,19 @@
         <v>0</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I124" s="2"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="5"/>
@@ -3341,36 +3369,36 @@
       <c r="G125" s="2">
         <v>0</v>
       </c>
-      <c r="H125" s="2"/>
+      <c r="H125" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="5"/>
-      <c r="F126" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G126" s="2"/>
-      <c r="H126" s="6" t="s">
-        <v>93</v>
-      </c>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2">
+        <v>0</v>
+      </c>
+      <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>10</v>
@@ -3378,108 +3406,172 @@
       <c r="D127" s="4"/>
       <c r="E127" s="5"/>
       <c r="F127" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G127" s="2"/>
       <c r="H127" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
+        <v>7</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128" s="4"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G128" s="2"/>
+      <c r="H128" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I128" s="2"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
         <v>8</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B129" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C128" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D128" s="4" t="s">
+      <c r="C129" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E128" s="5"/>
-      <c r="F128" s="6"/>
-      <c r="G128" s="2"/>
-      <c r="H128" s="6"/>
-      <c r="I128" s="2"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A129" s="103">
-        <v>9</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D129" s="4"/>
       <c r="E129" s="5"/>
       <c r="F129" s="6"/>
       <c r="G129" s="2"/>
       <c r="H129" s="6"/>
-      <c r="I129" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="I129" s="2"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="103">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="5"/>
       <c r="F130" s="6"/>
       <c r="G130" s="2"/>
       <c r="H130" s="6"/>
-      <c r="I130" s="2"/>
+      <c r="I130" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A131" s="2">
-        <v>11</v>
+      <c r="A131" s="103">
+        <v>10</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="5"/>
       <c r="F131" s="6"/>
       <c r="G131" s="2"/>
       <c r="H131" s="6"/>
-      <c r="I131" s="2" t="s">
-        <v>99</v>
+      <c r="I131" s="2"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>11</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D132" s="4"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="6"/>
+      <c r="I132" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A108:E108"/>
+    <mergeCell ref="A120:E120"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="A41:A51"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="A70:I71"/>
+    <mergeCell ref="E54:I54"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A32:A40"/>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A12:I13"/>
     <mergeCell ref="A24:I25"/>
-    <mergeCell ref="A82:I83"/>
-    <mergeCell ref="A95:I96"/>
-    <mergeCell ref="A107:E107"/>
-    <mergeCell ref="A119:E119"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="A40:A50"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="A69:I70"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="A58:A62"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A31:A39"/>
+    <mergeCell ref="A83:I84"/>
+    <mergeCell ref="A96:I97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B6:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
coding order model, route and page at frontend
</commit_message>
<xml_diff>
--- a/Database ToCoShop.xlsx
+++ b/Database ToCoShop.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="125">
   <si>
     <t>No.</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>Province</t>
-  </si>
-  <si>
-    <t>ShippingDuration</t>
   </si>
   <si>
     <t>CardHolder</t>
@@ -1339,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I133"/>
+  <dimension ref="A2:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1811,7 +1808,7 @@
         <v>32</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I28" s="10"/>
     </row>
@@ -1820,7 +1817,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>31</v>
@@ -1832,7 +1829,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I29" s="10"/>
     </row>
@@ -1841,7 +1838,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>31</v>
@@ -1853,7 +1850,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I30" s="10"/>
     </row>
@@ -1910,7 +1907,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I33" s="10"/>
     </row>
@@ -1931,7 +1928,7 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I34" s="10"/>
     </row>
@@ -2057,7 +2054,7 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="114"/>
       <c r="B42" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>10</v>
@@ -2122,7 +2119,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I45" s="10"/>
     </row>
@@ -2163,7 +2160,7 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="114"/>
       <c r="B48" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>14</v>
@@ -2180,7 +2177,7 @@
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="114"/>
       <c r="B49" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>14</v>
@@ -2212,9 +2209,9 @@
       <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="114"/>
+      <c r="A51" s="115"/>
       <c r="B51" s="10" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>14</v>
@@ -2230,194 +2227,190 @@
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="115"/>
-      <c r="B52" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="12">
-        <v>200</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-    </row>
-    <row r="53" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="113">
+    <row r="52" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="113">
         <v>7</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B52" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C52" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D52" s="15"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="114"/>
+      <c r="B53" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A54" s="114"/>
-      <c r="B54" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I54" s="10"/>
-    </row>
-    <row r="55" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B54" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" s="31"/>
+      <c r="E54" s="110" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="111"/>
+      <c r="G54" s="111"/>
+      <c r="H54" s="111"/>
+      <c r="I54" s="112"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="114"/>
-      <c r="B55" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D55" s="31"/>
-      <c r="E55" s="110" t="s">
-        <v>67</v>
-      </c>
-      <c r="F55" s="111"/>
-      <c r="G55" s="111"/>
-      <c r="H55" s="111"/>
-      <c r="I55" s="112"/>
+      <c r="B55" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="34"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="114"/>
       <c r="B56" s="32" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C56" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="34"/>
+      <c r="D56" s="34">
+        <v>50</v>
+      </c>
       <c r="E56" s="13"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
-      <c r="H56" s="14" t="s">
-        <v>104</v>
-      </c>
+      <c r="H56" s="10"/>
       <c r="I56" s="10"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="114"/>
       <c r="B57" s="32" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="34">
-        <v>50</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D57" s="34"/>
       <c r="E57" s="13"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
+      <c r="H57" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="114"/>
+      <c r="A58" s="115"/>
       <c r="B58" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D58" s="34"/>
+        <v>14</v>
+      </c>
+      <c r="D58" s="34">
+        <v>3</v>
+      </c>
       <c r="E58" s="13"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
-      <c r="H58" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="I58" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="115"/>
-      <c r="B59" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="34">
-        <v>3</v>
-      </c>
-      <c r="E59" s="13"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="104" t="s">
-        <v>103</v>
-      </c>
-      <c r="I59" s="10"/>
-    </row>
-    <row r="60" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="118">
+      <c r="H58" s="104" t="s">
+        <v>102</v>
+      </c>
+      <c r="I58" s="10"/>
+    </row>
+    <row r="59" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="118">
         <v>8</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B59" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="118"/>
+      <c r="B60" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G60" s="10"/>
+      <c r="H60" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I60" s="10"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="118"/>
       <c r="B61" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="13"/>
-      <c r="F61" s="14" t="s">
-        <v>35</v>
-      </c>
+      <c r="F61" s="10"/>
       <c r="G61" s="10"/>
-      <c r="H61" s="14" t="s">
-        <v>42</v>
-      </c>
+      <c r="H61" s="10"/>
       <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="118"/>
       <c r="B62" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="13"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
@@ -2426,10 +2419,10 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="118"/>
       <c r="B63" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
@@ -2439,36 +2432,40 @@
       <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="118"/>
-      <c r="B64" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
+      <c r="A64" s="113">
+        <v>9</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="113">
-        <v>9</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D65" s="15"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
+      <c r="A65" s="114"/>
+      <c r="B65" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" s="12"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="10"/>
+      <c r="H65" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="114"/>
@@ -2476,161 +2473,162 @@
         <v>110</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="13"/>
-      <c r="F66" s="14" t="s">
-        <v>35</v>
-      </c>
+      <c r="F66" s="14"/>
       <c r="G66" s="10"/>
       <c r="H66" s="14" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="I66" s="10"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="114"/>
+      <c r="A67" s="115"/>
       <c r="B67" s="10" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="12"/>
+      <c r="D67" s="12">
+        <v>500</v>
+      </c>
       <c r="E67" s="13"/>
-      <c r="F67" s="14"/>
+      <c r="F67" s="10"/>
       <c r="G67" s="10"/>
-      <c r="H67" s="14" t="s">
-        <v>112</v>
-      </c>
+      <c r="H67" s="10"/>
       <c r="I67" s="10"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="115"/>
-      <c r="B68" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="12">
-        <v>500</v>
-      </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="10"/>
-      <c r="I68" s="10"/>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="116" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="116"/>
+      <c r="C70" s="116"/>
+      <c r="D70" s="116"/>
+      <c r="E70" s="116"/>
+      <c r="F70" s="116"/>
+      <c r="G70" s="116"/>
+      <c r="H70" s="116"/>
+      <c r="I70" s="116"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="116" t="s">
-        <v>65</v>
-      </c>
-      <c r="B71" s="116"/>
-      <c r="C71" s="116"/>
-      <c r="D71" s="116"/>
-      <c r="E71" s="116"/>
-      <c r="F71" s="116"/>
-      <c r="G71" s="116"/>
-      <c r="H71" s="116"/>
-      <c r="I71" s="116"/>
+      <c r="A71" s="117"/>
+      <c r="B71" s="117"/>
+      <c r="C71" s="117"/>
+      <c r="D71" s="117"/>
+      <c r="E71" s="117"/>
+      <c r="F71" s="117"/>
+      <c r="G71" s="117"/>
+      <c r="H71" s="117"/>
+      <c r="I71" s="117"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="117"/>
-      <c r="B72" s="117"/>
-      <c r="C72" s="117"/>
-      <c r="D72" s="117"/>
-      <c r="E72" s="117"/>
-      <c r="F72" s="117"/>
-      <c r="G72" s="117"/>
-      <c r="H72" s="117"/>
-      <c r="I72" s="117"/>
+      <c r="A72" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G72" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="H72" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="45" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="45" t="s">
+      <c r="A73" s="46">
         <v>1</v>
       </c>
-      <c r="C73" s="45" t="s">
+      <c r="B73" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="48"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" s="46"/>
+      <c r="H73" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="I73" s="46"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="50">
+        <f>A73+1</f>
         <v>2</v>
       </c>
-      <c r="D73" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E73" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="F73" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="G73" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="H73" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="I73" s="45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="46">
-        <v>1</v>
-      </c>
-      <c r="B74" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D74" s="48"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="G74" s="46"/>
-      <c r="H74" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="I74" s="46"/>
+      <c r="B74" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="53">
+        <v>50</v>
+      </c>
+      <c r="E74" s="54"/>
+      <c r="F74" s="55"/>
+      <c r="G74" s="55"/>
+      <c r="H74" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I74" s="55"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="50">
         <f>A74+1</f>
-        <v>2</v>
-      </c>
-      <c r="B75" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="53">
-        <v>50</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B75" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="53"/>
       <c r="E75" s="54"/>
       <c r="F75" s="55"/>
       <c r="G75" s="55"/>
-      <c r="H75" s="50" t="s">
-        <v>15</v>
-      </c>
+      <c r="H75" s="50"/>
       <c r="I75" s="55"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="50">
-        <f>A75+1</f>
-        <v>3</v>
-      </c>
-      <c r="B76" s="64" t="s">
+      <c r="A76" s="105">
+        <f t="shared" ref="A76:A79" si="2">A75+1</f>
+        <v>4</v>
+      </c>
+      <c r="B76" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="D76" s="53"/>
+      <c r="C76" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="53">
+        <v>50</v>
+      </c>
       <c r="E76" s="54"/>
       <c r="F76" s="55"/>
       <c r="G76" s="55"/>
@@ -2638,11 +2636,11 @@
       <c r="I76" s="55"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="105">
-        <f t="shared" ref="A77:A80" si="2">A76+1</f>
-        <v>4</v>
-      </c>
-      <c r="B77" s="51" t="s">
+      <c r="A77" s="50">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B77" s="106" t="s">
         <v>107</v>
       </c>
       <c r="C77" s="52" t="s">
@@ -2651,155 +2649,157 @@
       <c r="D77" s="53">
         <v>50</v>
       </c>
-      <c r="E77" s="54"/>
-      <c r="F77" s="55"/>
-      <c r="G77" s="55"/>
+      <c r="E77" s="56"/>
+      <c r="F77" s="50"/>
+      <c r="G77" s="50"/>
       <c r="H77" s="50"/>
-      <c r="I77" s="55"/>
+      <c r="I77" s="50"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="50">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B78" s="106" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="C78" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="53">
+      <c r="C78" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="59">
         <v>50</v>
       </c>
-      <c r="E78" s="56"/>
-      <c r="F78" s="50"/>
-      <c r="G78" s="50"/>
-      <c r="H78" s="50"/>
-      <c r="I78" s="50"/>
+      <c r="E78" s="60"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="61"/>
+      <c r="H78" s="61"/>
+      <c r="I78" s="61"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="50">
         <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B79" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="63">
+        <v>200</v>
+      </c>
+      <c r="E79" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="50"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="119" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="119"/>
+      <c r="C83" s="119"/>
+      <c r="D83" s="119"/>
+      <c r="E83" s="119"/>
+      <c r="F83" s="119"/>
+      <c r="G83" s="119"/>
+      <c r="H83" s="119"/>
+      <c r="I83" s="119"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="122"/>
+      <c r="B84" s="122"/>
+      <c r="C84" s="122"/>
+      <c r="D84" s="122"/>
+      <c r="E84" s="122"/>
+      <c r="F84" s="122"/>
+      <c r="G84" s="122"/>
+      <c r="H84" s="122"/>
+      <c r="I84" s="122"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C79" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" s="59">
+      <c r="H85" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="40">
+        <v>1</v>
+      </c>
+      <c r="B86" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" s="42"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G86" s="40"/>
+      <c r="H86" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I86" s="44"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="36">
+        <f>A86+1</f>
+        <v>2</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="37">
         <v>50</v>
       </c>
-      <c r="E79" s="60"/>
-      <c r="F79" s="61"/>
-      <c r="G79" s="61"/>
-      <c r="H79" s="61"/>
-      <c r="I79" s="61"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="50">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="B80" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="C80" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="63">
-        <v>200</v>
-      </c>
-      <c r="E80" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F80" s="50"/>
-      <c r="G80" s="50"/>
-      <c r="H80" s="50"/>
-      <c r="I80" s="50"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="119" t="s">
-        <v>68</v>
-      </c>
-      <c r="B84" s="119"/>
-      <c r="C84" s="119"/>
-      <c r="D84" s="119"/>
-      <c r="E84" s="119"/>
-      <c r="F84" s="119"/>
-      <c r="G84" s="119"/>
-      <c r="H84" s="119"/>
-      <c r="I84" s="119"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="122"/>
-      <c r="B85" s="122"/>
-      <c r="C85" s="122"/>
-      <c r="D85" s="122"/>
-      <c r="E85" s="122"/>
-      <c r="F85" s="122"/>
-      <c r="G85" s="122"/>
-      <c r="H85" s="122"/>
-      <c r="I85" s="122"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D86" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E86" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="F86" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="G86" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="H86" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="I86" s="39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="40">
-        <v>1</v>
-      </c>
-      <c r="B87" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C87" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D87" s="42"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G87" s="40"/>
-      <c r="H87" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="I87" s="44"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="I87" s="36"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="36">
-        <f>A87+1</f>
-        <v>2</v>
+        <f t="shared" ref="A88:A90" si="3">A87+1</f>
+        <v>3</v>
       </c>
       <c r="B88" s="36" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="C88" s="35" t="s">
         <v>14</v>
@@ -2810,324 +2810,321 @@
       <c r="E88" s="38"/>
       <c r="F88" s="36"/>
       <c r="G88" s="36"/>
-      <c r="H88" s="68" t="s">
-        <v>71</v>
-      </c>
+      <c r="H88" s="36"/>
       <c r="I88" s="36"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="36">
-        <f t="shared" ref="A89:A91" si="3">A88+1</f>
-        <v>3</v>
-      </c>
-      <c r="B89" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C89" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D89" s="37">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="28">
         <v>50</v>
       </c>
-      <c r="E89" s="38"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="36"/>
-      <c r="H89" s="36"/>
-      <c r="I89" s="36"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H89" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I89" s="24"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="36">
         <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B90" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="37"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="36"/>
+      <c r="G90" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H90" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I90" s="36"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="67"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="119" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" s="119"/>
+      <c r="C96" s="119"/>
+      <c r="D96" s="119"/>
+      <c r="E96" s="119"/>
+      <c r="F96" s="119"/>
+      <c r="G96" s="119"/>
+      <c r="H96" s="119"/>
+      <c r="I96" s="119"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="122"/>
+      <c r="B97" s="122"/>
+      <c r="C97" s="122"/>
+      <c r="D97" s="122"/>
+      <c r="E97" s="122"/>
+      <c r="F97" s="122"/>
+      <c r="G97" s="122"/>
+      <c r="H97" s="122"/>
+      <c r="I97" s="122"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C90" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" s="28">
+      <c r="F98" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H98" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I98" s="39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="40">
+        <v>1</v>
+      </c>
+      <c r="B99" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="42"/>
+      <c r="E99" s="43"/>
+      <c r="F99" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G99" s="40"/>
+      <c r="H99" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I99" s="44"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="36">
+        <f>A99+1</f>
+        <v>2</v>
+      </c>
+      <c r="B100" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" s="37">
         <v>50</v>
       </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H90" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="I90" s="24"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="36">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="B91" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C91" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="D91" s="37"/>
-      <c r="E91" s="38"/>
-      <c r="F91" s="36"/>
-      <c r="G91" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="H91" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="I91" s="36"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="67"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="119" t="s">
-        <v>78</v>
-      </c>
-      <c r="B97" s="119"/>
-      <c r="C97" s="119"/>
-      <c r="D97" s="119"/>
-      <c r="E97" s="119"/>
-      <c r="F97" s="119"/>
-      <c r="G97" s="119"/>
-      <c r="H97" s="119"/>
-      <c r="I97" s="119"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="122"/>
-      <c r="B98" s="122"/>
-      <c r="C98" s="122"/>
-      <c r="D98" s="122"/>
-      <c r="E98" s="122"/>
-      <c r="F98" s="122"/>
-      <c r="G98" s="122"/>
-      <c r="H98" s="122"/>
-      <c r="I98" s="122"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B99" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D99" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E99" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="F99" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="G99" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="H99" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="I99" s="39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="40">
-        <v>1</v>
-      </c>
-      <c r="B100" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C100" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D100" s="42"/>
-      <c r="E100" s="43"/>
-      <c r="F100" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G100" s="40"/>
-      <c r="H100" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="I100" s="44"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="36"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="68"/>
+      <c r="I100" s="36"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="36">
-        <f>A100+1</f>
-        <v>2</v>
+        <f t="shared" ref="A101:A103" si="4">A100+1</f>
+        <v>3</v>
       </c>
       <c r="B101" s="36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C101" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D101" s="37">
-        <v>50</v>
-      </c>
-      <c r="E101" s="38"/>
+        <v>500</v>
+      </c>
+      <c r="E101" s="38" t="s">
+        <v>17</v>
+      </c>
       <c r="F101" s="36"/>
       <c r="G101" s="36"/>
-      <c r="H101" s="68"/>
+      <c r="H101" s="36"/>
       <c r="I101" s="36"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="36">
-        <f t="shared" ref="A102:A104" si="4">A101+1</f>
-        <v>3</v>
-      </c>
-      <c r="B102" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C102" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" s="37">
-        <v>500</v>
-      </c>
-      <c r="E102" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F102" s="36"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="36"/>
-      <c r="I102" s="36"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="36">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B103" s="27" t="s">
+      <c r="B102" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C103" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" s="28" t="s">
+      <c r="C102" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E103" s="8"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="24"/>
-      <c r="H103" s="24"/>
-      <c r="I103" s="24"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="69">
+      <c r="E102" s="8"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="69">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B104" s="69" t="s">
+      <c r="B103" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="C104" s="70" t="s">
+      <c r="C103" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="D104" s="71"/>
-      <c r="E104" s="72"/>
-      <c r="F104" s="69"/>
-      <c r="G104" s="73"/>
-      <c r="H104" s="73"/>
-      <c r="I104" s="69"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="74">
+      <c r="D103" s="71"/>
+      <c r="E103" s="72"/>
+      <c r="F103" s="69"/>
+      <c r="G103" s="73"/>
+      <c r="H103" s="73"/>
+      <c r="I103" s="69"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="74">
         <v>6</v>
       </c>
-      <c r="B105" s="74" t="s">
+      <c r="B104" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C105" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D105" s="74"/>
-      <c r="E105" s="74"/>
-      <c r="F105" s="74"/>
-      <c r="G105" s="75" t="s">
+      <c r="C104" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="74"/>
+      <c r="G104" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="H105" s="75" t="s">
+      <c r="H104" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="I105" s="74"/>
+      <c r="I104" s="74"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="107" t="s">
+        <v>83</v>
+      </c>
+      <c r="B108" s="108"/>
+      <c r="C108" s="108"/>
+      <c r="D108" s="108"/>
+      <c r="E108" s="108"/>
+      <c r="F108" s="77"/>
+      <c r="G108" s="77"/>
+      <c r="H108" s="77"/>
+      <c r="I108" s="77"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="107" t="s">
-        <v>83</v>
-      </c>
-      <c r="B109" s="108"/>
-      <c r="C109" s="108"/>
-      <c r="D109" s="108"/>
-      <c r="E109" s="108"/>
-      <c r="F109" s="77"/>
-      <c r="G109" s="77"/>
-      <c r="H109" s="77"/>
-      <c r="I109" s="77"/>
+      <c r="A109" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="F109" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="G109" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="H109" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="I109" s="78" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="78" t="s">
+      <c r="A110" s="79">
         <v>1</v>
       </c>
-      <c r="C110" s="78" t="s">
+      <c r="B110" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110" s="81">
+        <v>50</v>
+      </c>
+      <c r="E110" s="82"/>
+      <c r="F110" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G110" s="79"/>
+      <c r="H110" s="79"/>
+      <c r="I110" s="79"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="83">
         <v>2</v>
       </c>
-      <c r="D110" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="E110" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="F110" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="G110" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="H110" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="I110" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="79">
-        <v>1</v>
-      </c>
-      <c r="B111" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111" s="80" t="s">
-        <v>10</v>
-      </c>
-      <c r="D111" s="81">
+      <c r="B111" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C111" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" s="85">
         <v>50</v>
       </c>
-      <c r="E111" s="82"/>
-      <c r="F111" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="G111" s="79"/>
-      <c r="H111" s="79"/>
-      <c r="I111" s="79"/>
+      <c r="E111" s="86"/>
+      <c r="F111" s="83"/>
+      <c r="G111" s="83"/>
+      <c r="H111" s="83"/>
+      <c r="I111" s="83"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="83">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B112" s="83" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C112" s="84" t="s">
         <v>14</v>
@@ -3143,10 +3140,10 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="83">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B113" s="83" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="C113" s="84" t="s">
         <v>14</v>
@@ -3154,7 +3151,9 @@
       <c r="D113" s="85">
         <v>50</v>
       </c>
-      <c r="E113" s="86"/>
+      <c r="E113" s="86" t="s">
+        <v>17</v>
+      </c>
       <c r="F113" s="83"/>
       <c r="G113" s="83"/>
       <c r="H113" s="83"/>
@@ -3162,20 +3161,18 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="83">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B114" s="83" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C114" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D114" s="85">
-        <v>50</v>
-      </c>
-      <c r="E114" s="86" t="s">
-        <v>17</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="E114" s="86"/>
       <c r="F114" s="83"/>
       <c r="G114" s="83"/>
       <c r="H114" s="83"/>
@@ -3183,62 +3180,54 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="83">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B115" s="83" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C115" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D115" s="85">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="E115" s="86"/>
       <c r="F115" s="83"/>
       <c r="G115" s="83"/>
-      <c r="H115" s="83"/>
+      <c r="H115" s="83" t="s">
+        <v>15</v>
+      </c>
       <c r="I115" s="83"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="83">
-        <v>6</v>
-      </c>
-      <c r="B116" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="C116" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D116" s="85">
-        <v>50</v>
-      </c>
-      <c r="E116" s="86"/>
-      <c r="F116" s="83"/>
-      <c r="G116" s="83"/>
-      <c r="H116" s="83" t="s">
-        <v>15</v>
-      </c>
-      <c r="I116" s="83"/>
+      <c r="A116" s="98">
+        <v>7</v>
+      </c>
+      <c r="B116" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="C116" s="99" t="s">
+        <v>31</v>
+      </c>
+      <c r="D116" s="100"/>
+      <c r="E116" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="F116" s="98"/>
+      <c r="G116" s="98"/>
+      <c r="H116" s="98"/>
+      <c r="I116" s="98"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="98">
-        <v>7</v>
-      </c>
-      <c r="B117" s="98" t="s">
-        <v>85</v>
-      </c>
-      <c r="C117" s="99" t="s">
-        <v>31</v>
-      </c>
-      <c r="D117" s="100"/>
-      <c r="E117" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="F117" s="98"/>
-      <c r="G117" s="98"/>
-      <c r="H117" s="98"/>
-      <c r="I117" s="98"/>
+      <c r="A117" s="94"/>
+      <c r="B117" s="94"/>
+      <c r="C117" s="95"/>
+      <c r="D117" s="96"/>
+      <c r="E117" s="97"/>
+      <c r="F117" s="94"/>
+      <c r="G117" s="94"/>
+      <c r="H117" s="94"/>
+      <c r="I117" s="94"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="94"/>
@@ -3252,115 +3241,125 @@
       <c r="I118" s="94"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="94"/>
-      <c r="B119" s="94"/>
-      <c r="C119" s="95"/>
-      <c r="D119" s="96"/>
-      <c r="E119" s="97"/>
-      <c r="F119" s="94"/>
-      <c r="G119" s="94"/>
-      <c r="H119" s="94"/>
-      <c r="I119" s="94"/>
+      <c r="A119" s="102"/>
+      <c r="B119" s="102"/>
+      <c r="C119" s="102"/>
+      <c r="D119" s="102"/>
+      <c r="E119" s="102"/>
+      <c r="F119" s="102"/>
+      <c r="G119" s="102"/>
+      <c r="H119" s="102"/>
+      <c r="I119" s="102"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="102"/>
-      <c r="B120" s="102"/>
-      <c r="C120" s="102"/>
-      <c r="D120" s="102"/>
-      <c r="E120" s="102"/>
-      <c r="F120" s="102"/>
-      <c r="G120" s="102"/>
-      <c r="H120" s="102"/>
-      <c r="I120" s="102"/>
+      <c r="A120" s="109" t="s">
+        <v>86</v>
+      </c>
+      <c r="B120" s="108"/>
+      <c r="C120" s="108"/>
+      <c r="D120" s="108"/>
+      <c r="E120" s="108"/>
+      <c r="F120" s="87"/>
+      <c r="G120" s="87"/>
+      <c r="H120" s="87"/>
+      <c r="I120" s="87"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="109" t="s">
-        <v>86</v>
-      </c>
-      <c r="B121" s="108"/>
-      <c r="C121" s="108"/>
-      <c r="D121" s="108"/>
-      <c r="E121" s="108"/>
-      <c r="F121" s="87"/>
-      <c r="G121" s="87"/>
-      <c r="H121" s="87"/>
-      <c r="I121" s="87"/>
+      <c r="A121" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="E121" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F121" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="G121" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="H121" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="I121" s="88" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B122" s="88" t="s">
+      <c r="A122" s="1">
         <v>1</v>
       </c>
-      <c r="C122" s="88" t="s">
+      <c r="B122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" s="90"/>
+      <c r="E122" s="91"/>
+      <c r="F122" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
         <v>2</v>
       </c>
-      <c r="D122" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="E122" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="F122" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="G122" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="H122" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="I122" s="88" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="1">
-        <v>1</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C123" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="D123" s="90"/>
-      <c r="E123" s="91"/>
-      <c r="F123" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I123" s="1"/>
+      <c r="B123" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" s="92">
+        <v>50</v>
+      </c>
+      <c r="E123" s="93"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D124" s="92">
-        <v>50</v>
-      </c>
-      <c r="E124" s="93"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="6"/>
-      <c r="H124" s="6"/>
-      <c r="I124" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2">
+        <v>0</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I124" s="2"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>44</v>
@@ -3372,16 +3371,16 @@
         <v>0</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>44</v>
@@ -3392,36 +3391,36 @@
       <c r="G126" s="2">
         <v>0</v>
       </c>
-      <c r="H126" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="5"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2">
-        <v>0</v>
-      </c>
-      <c r="H127" s="2"/>
+      <c r="F127" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G127" s="2"/>
+      <c r="H127" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>10</v>
@@ -3433,102 +3432,81 @@
       </c>
       <c r="G128" s="2"/>
       <c r="H128" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I128" s="2"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D129" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="E129" s="5"/>
-      <c r="F129" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="F129" s="6"/>
       <c r="G129" s="2"/>
-      <c r="H129" s="6" t="s">
-        <v>93</v>
-      </c>
+      <c r="H129" s="6"/>
       <c r="I129" s="2"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" s="2">
-        <v>8</v>
+      <c r="A130" s="103">
+        <v>9</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D130" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" s="4"/>
       <c r="E130" s="5"/>
       <c r="F130" s="6"/>
       <c r="G130" s="2"/>
       <c r="H130" s="6"/>
-      <c r="I130" s="2"/>
+      <c r="I130" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="103">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="5"/>
       <c r="F131" s="6"/>
       <c r="G131" s="2"/>
       <c r="H131" s="6"/>
-      <c r="I131" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="I131" s="2"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A132" s="103">
-        <v>10</v>
+      <c r="A132" s="2">
+        <v>11</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>14</v>
+        <v>95</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="5"/>
       <c r="F132" s="6"/>
       <c r="G132" s="2"/>
       <c r="H132" s="6"/>
-      <c r="I132" s="2"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="2">
-        <v>11</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D133" s="4"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="6"/>
-      <c r="G133" s="2"/>
-      <c r="H133" s="6"/>
-      <c r="I133" s="2" t="s">
+      <c r="I132" s="2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3537,18 +3515,18 @@
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A12:I13"/>
     <mergeCell ref="A24:I25"/>
-    <mergeCell ref="A84:I85"/>
-    <mergeCell ref="A97:I98"/>
-    <mergeCell ref="A109:E109"/>
-    <mergeCell ref="A121:E121"/>
+    <mergeCell ref="A83:I84"/>
+    <mergeCell ref="A96:I97"/>
+    <mergeCell ref="A108:E108"/>
+    <mergeCell ref="A120:E120"/>
     <mergeCell ref="E37:I37"/>
-    <mergeCell ref="A41:A52"/>
+    <mergeCell ref="A41:A51"/>
     <mergeCell ref="E46:I46"/>
-    <mergeCell ref="A71:I72"/>
-    <mergeCell ref="E55:I55"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A70:I71"/>
+    <mergeCell ref="E54:I54"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="A64:A67"/>
     <mergeCell ref="A32:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3576,22 +3554,22 @@
   <sheetData>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
         <v>113</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="s">
         <v>114</v>
       </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>117</v>
-      </c>
-      <c r="F6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continue to config Order
</commit_message>
<xml_diff>
--- a/Database ToCoShop.xlsx
+++ b/Database ToCoShop.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="127">
   <si>
     <t>No.</t>
   </si>
@@ -140,9 +140,6 @@
     <t>PaymentInfo</t>
   </si>
   <si>
-    <t>Reference Products (Id)</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t xml:space="preserve"> Object</t>
   </si>
   <si>
-    <t>Address is one field in ContactInfo</t>
-  </si>
-  <si>
     <t>COLLECTION: Transportations</t>
   </si>
   <si>
@@ -390,6 +384,18 @@
   </si>
   <si>
     <t>ProductId</t>
+  </si>
+  <si>
+    <t>ObjectId</t>
+  </si>
+  <si>
+    <t>Reference Products (id)</t>
+  </si>
+  <si>
+    <t>[0,1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>ngay chuyen hang co the la ngay mai hay phai la hom nay hoac qua khu</t>
   </si>
 </sst>
 </file>
@@ -740,7 +746,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -984,24 +990,9 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1009,6 +1000,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1018,17 +1024,20 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1336,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I133"/>
+  <dimension ref="A2:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1357,28 +1366,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
     </row>
     <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
+      <c r="A3" s="123"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
     </row>
     <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -1519,28 +1528,28 @@
       <c r="I9" s="24"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="109" t="s">
+      <c r="A12" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="109"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
+      <c r="A13" s="117"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
@@ -1717,28 +1726,28 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="111" t="s">
+      <c r="A24" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="124"/>
+      <c r="E24" s="124"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="124"/>
+      <c r="I24" s="124"/>
     </row>
     <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="111"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="111"/>
-      <c r="I25" s="111"/>
+      <c r="A25" s="124"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="124"/>
+      <c r="D25" s="124"/>
+      <c r="E25" s="124"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="124"/>
+      <c r="I25" s="124"/>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -1808,7 +1817,7 @@
         <v>32</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I28" s="10"/>
     </row>
@@ -1817,7 +1826,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>31</v>
@@ -1829,7 +1838,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I29" s="10"/>
     </row>
@@ -1838,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>31</v>
@@ -1850,7 +1859,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I30" s="10"/>
     </row>
@@ -1871,12 +1880,12 @@
         <v>34</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="119">
+      <c r="A32" s="113">
         <v>5</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -1893,7 +1902,7 @@
       <c r="I32" s="14"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="120"/>
+      <c r="A33" s="114"/>
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
@@ -1907,12 +1916,12 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="120"/>
+      <c r="A34" s="114"/>
       <c r="B34" s="10" t="s">
         <v>25</v>
       </c>
@@ -1928,14 +1937,14 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="120"/>
+      <c r="A35" s="114"/>
       <c r="B35" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>14</v>
@@ -1946,15 +1955,15 @@
       <c r="E35" s="13"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="120"/>
+      <c r="A36" s="114"/>
       <c r="B36" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>14</v>
@@ -1965,32 +1974,32 @@
       <c r="E36" s="13"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A37" s="120"/>
+      <c r="A37" s="114"/>
       <c r="B37" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="31"/>
-      <c r="E37" s="116" t="s">
-        <v>63</v>
-      </c>
-      <c r="F37" s="117"/>
-      <c r="G37" s="117"/>
-      <c r="H37" s="117"/>
-      <c r="I37" s="118"/>
+      <c r="E37" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="108"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="108"/>
+      <c r="I37" s="109"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="120"/>
+      <c r="A38" s="114"/>
       <c r="B38" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>14</v>
@@ -2007,9 +2016,9 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="120"/>
+      <c r="A39" s="114"/>
       <c r="B39" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>14</v>
@@ -2026,9 +2035,9 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="120"/>
+      <c r="A40" s="114"/>
       <c r="B40" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>14</v>
@@ -2045,9 +2054,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="121"/>
+      <c r="A41" s="115"/>
       <c r="B41" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>14</v>
@@ -2058,13 +2067,13 @@
       <c r="E41" s="13"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="119">
+      <c r="A42" s="113">
         <v>6</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -2074,16 +2083,18 @@
         <v>38</v>
       </c>
       <c r="D42" s="15"/>
-      <c r="E42" s="16"/>
+      <c r="E42" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="120"/>
+      <c r="A43" s="114"/>
       <c r="B43" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>10</v>
@@ -2095,14 +2106,14 @@
       </c>
       <c r="G43" s="10"/>
       <c r="H43" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="120"/>
+      <c r="A44" s="114"/>
       <c r="B44" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>14</v>
@@ -2113,15 +2124,15 @@
       <c r="E44" s="13"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="120"/>
+      <c r="A45" s="114"/>
       <c r="B45" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>14</v>
@@ -2132,13 +2143,13 @@
       <c r="E45" s="13"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="120"/>
+      <c r="A46" s="114"/>
       <c r="B46" s="10" t="s">
         <v>26</v>
       </c>
@@ -2148,37 +2159,37 @@
       <c r="D46" s="12">
         <v>50</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="E46" s="13"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A47" s="120"/>
+      <c r="A47" s="114"/>
       <c r="B47" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="31"/>
-      <c r="E47" s="116" t="s">
-        <v>76</v>
-      </c>
-      <c r="F47" s="117"/>
-      <c r="G47" s="117"/>
-      <c r="H47" s="117"/>
-      <c r="I47" s="118"/>
+      <c r="E47" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="119" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="119"/>
+      <c r="H47" s="119"/>
+      <c r="I47" s="120"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="120"/>
+      <c r="A48" s="114"/>
       <c r="B48" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>14</v>
@@ -2195,9 +2206,9 @@
       <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="120"/>
+      <c r="A49" s="114"/>
       <c r="B49" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>14</v>
@@ -2214,9 +2225,9 @@
       <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="120"/>
+      <c r="A50" s="114"/>
       <c r="B50" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>14</v>
@@ -2233,9 +2244,9 @@
       <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="120"/>
+      <c r="A51" s="114"/>
       <c r="B51" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>14</v>
@@ -2246,15 +2257,15 @@
       <c r="E51" s="13"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="121"/>
+      <c r="A52" s="115"/>
       <c r="B52" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>14</v>
@@ -2271,7 +2282,7 @@
       <c r="I52" s="10"/>
     </row>
     <row r="53" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="119">
+      <c r="A53" s="113">
         <v>7</v>
       </c>
       <c r="B53" s="14" t="s">
@@ -2290,9 +2301,9 @@
       <c r="I53" s="14"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="120"/>
+      <c r="A54" s="114"/>
       <c r="B54" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>14</v>
@@ -2302,31 +2313,31 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54" s="10"/>
+    </row>
+    <row r="55" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A55" s="114"/>
+      <c r="B55" s="29" t="s">
         <v>57</v>
-      </c>
-      <c r="I54" s="10"/>
-    </row>
-    <row r="55" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A55" s="120"/>
-      <c r="B55" s="29" t="s">
-        <v>58</v>
       </c>
       <c r="C55" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D55" s="31"/>
-      <c r="E55" s="116" t="s">
-        <v>66</v>
-      </c>
-      <c r="F55" s="117"/>
-      <c r="G55" s="117"/>
-      <c r="H55" s="117"/>
-      <c r="I55" s="118"/>
+      <c r="E55" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55" s="119"/>
+      <c r="G55" s="119"/>
+      <c r="H55" s="119"/>
+      <c r="I55" s="120"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="120"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56" s="33" t="s">
         <v>14</v>
@@ -2336,14 +2347,14 @@
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I56" s="10"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="120"/>
+      <c r="A57" s="114"/>
       <c r="B57" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C57" s="33" t="s">
         <v>14</v>
@@ -2358,9 +2369,9 @@
       <c r="I57" s="10"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="120"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>31</v>
@@ -2370,16 +2381,16 @@
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="121"/>
+      <c r="A59" s="115"/>
       <c r="B59" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="33" t="s">
         <v>14</v>
@@ -2391,19 +2402,19 @@
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I59" s="10"/>
     </row>
     <row r="60" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="122">
+      <c r="A60" s="121">
         <v>8</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
@@ -2413,12 +2424,12 @@
       <c r="I60" s="14"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="122"/>
+      <c r="A61" s="121"/>
       <c r="B61" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="13"/>
@@ -2427,17 +2438,17 @@
       </c>
       <c r="G61" s="10"/>
       <c r="H61" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I61" s="10"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="121"/>
+      <c r="B62" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I61" s="10"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="122"/>
-      <c r="B62" s="10" t="s">
+      <c r="C62" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
@@ -2447,12 +2458,12 @@
       <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="122"/>
+      <c r="A63" s="121"/>
       <c r="B63" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="13"/>
@@ -2462,12 +2473,12 @@
       <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="122"/>
+      <c r="A64" s="121"/>
       <c r="B64" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="13"/>
@@ -2477,26 +2488,26 @@
       <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="119">
+      <c r="A65" s="113">
         <v>9</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D65" s="15"/>
-      <c r="E65" s="16"/>
+      <c r="E65" s="13"/>
       <c r="F65" s="14"/>
       <c r="G65" s="14"/>
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="120"/>
+      <c r="A66" s="114"/>
       <c r="B66" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>10</v>
@@ -2513,26 +2524,28 @@
       <c r="I66" s="10"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="120"/>
+      <c r="A67" s="114"/>
       <c r="B67" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="12"/>
+      <c r="D67" s="12">
+        <v>50</v>
+      </c>
       <c r="E67" s="13"/>
       <c r="F67" s="14"/>
       <c r="G67" s="10"/>
       <c r="H67" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I67" s="10"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="121"/>
+      <c r="A68" s="115"/>
       <c r="B68" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C68" s="11" t="s">
         <v>14</v>
@@ -2547,28 +2560,28 @@
       <c r="I68" s="10"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="109" t="s">
-        <v>64</v>
-      </c>
-      <c r="B71" s="109"/>
-      <c r="C71" s="109"/>
-      <c r="D71" s="109"/>
-      <c r="E71" s="109"/>
-      <c r="F71" s="109"/>
-      <c r="G71" s="109"/>
-      <c r="H71" s="109"/>
-      <c r="I71" s="109"/>
+      <c r="A71" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="116"/>
+      <c r="C71" s="116"/>
+      <c r="D71" s="116"/>
+      <c r="E71" s="116"/>
+      <c r="F71" s="116"/>
+      <c r="G71" s="116"/>
+      <c r="H71" s="116"/>
+      <c r="I71" s="116"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="110"/>
-      <c r="B72" s="110"/>
-      <c r="C72" s="110"/>
-      <c r="D72" s="110"/>
-      <c r="E72" s="110"/>
-      <c r="F72" s="110"/>
-      <c r="G72" s="110"/>
-      <c r="H72" s="110"/>
-      <c r="I72" s="110"/>
+      <c r="A72" s="117"/>
+      <c r="B72" s="117"/>
+      <c r="C72" s="117"/>
+      <c r="D72" s="117"/>
+      <c r="E72" s="117"/>
+      <c r="F72" s="117"/>
+      <c r="G72" s="117"/>
+      <c r="H72" s="117"/>
+      <c r="I72" s="117"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="45" t="s">
@@ -2648,10 +2661,10 @@
         <v>3</v>
       </c>
       <c r="B76" s="64" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C76" s="65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D76" s="53"/>
       <c r="E76" s="54"/>
@@ -2666,7 +2679,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C77" s="52" t="s">
         <v>14</v>
@@ -2686,7 +2699,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="106" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C78" s="52" t="s">
         <v>14</v>
@@ -2706,7 +2719,7 @@
         <v>6</v>
       </c>
       <c r="B79" s="57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C79" s="58" t="s">
         <v>14</v>
@@ -2726,7 +2739,7 @@
         <v>7</v>
       </c>
       <c r="B80" s="50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C80" s="62" t="s">
         <v>14</v>
@@ -2743,28 +2756,28 @@
       <c r="I80" s="50"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="107" t="s">
-        <v>67</v>
-      </c>
-      <c r="B84" s="107"/>
-      <c r="C84" s="107"/>
-      <c r="D84" s="107"/>
-      <c r="E84" s="107"/>
-      <c r="F84" s="107"/>
-      <c r="G84" s="107"/>
-      <c r="H84" s="107"/>
-      <c r="I84" s="107"/>
+      <c r="A84" s="122" t="s">
+        <v>65</v>
+      </c>
+      <c r="B84" s="122"/>
+      <c r="C84" s="122"/>
+      <c r="D84" s="122"/>
+      <c r="E84" s="122"/>
+      <c r="F84" s="122"/>
+      <c r="G84" s="122"/>
+      <c r="H84" s="122"/>
+      <c r="I84" s="122"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="112"/>
-      <c r="B85" s="112"/>
-      <c r="C85" s="112"/>
-      <c r="D85" s="112"/>
-      <c r="E85" s="112"/>
-      <c r="F85" s="112"/>
-      <c r="G85" s="112"/>
-      <c r="H85" s="112"/>
-      <c r="I85" s="112"/>
+      <c r="A85" s="125"/>
+      <c r="B85" s="125"/>
+      <c r="C85" s="125"/>
+      <c r="D85" s="125"/>
+      <c r="E85" s="125"/>
+      <c r="F85" s="125"/>
+      <c r="G85" s="125"/>
+      <c r="H85" s="125"/>
+      <c r="I85" s="125"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="39" t="s">
@@ -2841,7 +2854,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C89" s="35" t="s">
         <v>14</v>
@@ -2872,10 +2885,10 @@
       <c r="E90" s="8"/>
       <c r="F90" s="24"/>
       <c r="G90" s="24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H90" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I90" s="24"/>
     </row>
@@ -2885,19 +2898,19 @@
         <v>5</v>
       </c>
       <c r="B91" s="36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C91" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="38"/>
       <c r="F91" s="36"/>
       <c r="G91" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H91" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I91" s="36"/>
     </row>
@@ -2905,28 +2918,28 @@
       <c r="A93" s="67"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="107" t="s">
-        <v>77</v>
-      </c>
-      <c r="B97" s="107"/>
-      <c r="C97" s="107"/>
-      <c r="D97" s="107"/>
-      <c r="E97" s="107"/>
-      <c r="F97" s="107"/>
-      <c r="G97" s="107"/>
-      <c r="H97" s="107"/>
-      <c r="I97" s="107"/>
+      <c r="A97" s="122" t="s">
+        <v>75</v>
+      </c>
+      <c r="B97" s="122"/>
+      <c r="C97" s="122"/>
+      <c r="D97" s="122"/>
+      <c r="E97" s="122"/>
+      <c r="F97" s="122"/>
+      <c r="G97" s="122"/>
+      <c r="H97" s="122"/>
+      <c r="I97" s="122"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="112"/>
-      <c r="B98" s="112"/>
-      <c r="C98" s="112"/>
-      <c r="D98" s="112"/>
-      <c r="E98" s="112"/>
-      <c r="F98" s="112"/>
-      <c r="G98" s="112"/>
-      <c r="H98" s="112"/>
-      <c r="I98" s="112"/>
+      <c r="A98" s="125"/>
+      <c r="B98" s="125"/>
+      <c r="C98" s="125"/>
+      <c r="D98" s="125"/>
+      <c r="E98" s="125"/>
+      <c r="F98" s="125"/>
+      <c r="G98" s="125"/>
+      <c r="H98" s="125"/>
+      <c r="I98" s="125"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="39" t="s">
@@ -2984,7 +2997,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C101" s="35" t="s">
         <v>14</v>
@@ -3004,7 +3017,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C102" s="35" t="s">
         <v>14</v>
@@ -3046,16 +3059,18 @@
         <v>5</v>
       </c>
       <c r="B104" s="69" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C104" s="70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D104" s="71"/>
       <c r="E104" s="72"/>
       <c r="F104" s="69"/>
       <c r="G104" s="73"/>
-      <c r="H104" s="73"/>
+      <c r="H104" s="73" t="s">
+        <v>125</v>
+      </c>
       <c r="I104" s="69"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
@@ -3072,21 +3087,21 @@
       <c r="E105" s="74"/>
       <c r="F105" s="74"/>
       <c r="G105" s="75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H105" s="75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I105" s="74"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="113" t="s">
-        <v>82</v>
-      </c>
-      <c r="B109" s="114"/>
-      <c r="C109" s="114"/>
-      <c r="D109" s="114"/>
-      <c r="E109" s="114"/>
+      <c r="A109" s="110" t="s">
+        <v>80</v>
+      </c>
+      <c r="B109" s="111"/>
+      <c r="C109" s="111"/>
+      <c r="D109" s="111"/>
+      <c r="E109" s="111"/>
       <c r="F109" s="77"/>
       <c r="G109" s="77"/>
       <c r="H109" s="77"/>
@@ -3147,7 +3162,7 @@
         <v>2</v>
       </c>
       <c r="B112" s="83" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C112" s="84" t="s">
         <v>14</v>
@@ -3166,7 +3181,7 @@
         <v>3</v>
       </c>
       <c r="B113" s="83" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C113" s="84" t="s">
         <v>14</v>
@@ -3218,7 +3233,7 @@
       <c r="F115" s="83"/>
       <c r="G115" s="83"/>
       <c r="H115" s="68" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I115" s="83"/>
     </row>
@@ -3248,7 +3263,7 @@
         <v>7</v>
       </c>
       <c r="B117" s="98" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C117" s="99" t="s">
         <v>31</v>
@@ -3296,13 +3311,13 @@
       <c r="I120" s="102"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="115" t="s">
-        <v>85</v>
-      </c>
-      <c r="B121" s="114"/>
-      <c r="C121" s="114"/>
-      <c r="D121" s="114"/>
-      <c r="E121" s="114"/>
+      <c r="A121" s="112" t="s">
+        <v>83</v>
+      </c>
+      <c r="B121" s="111"/>
+      <c r="C121" s="111"/>
+      <c r="D121" s="111"/>
+      <c r="E121" s="111"/>
       <c r="F121" s="87"/>
       <c r="G121" s="87"/>
       <c r="H121" s="87"/>
@@ -3382,10 +3397,10 @@
         <v>3</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="5"/>
@@ -3394,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I125" s="2"/>
     </row>
@@ -3403,10 +3418,10 @@
         <v>4</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="5"/>
@@ -3415,7 +3430,7 @@
         <v>0</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I126" s="2"/>
     </row>
@@ -3424,10 +3439,10 @@
         <v>5</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="5"/>
@@ -3443,7 +3458,7 @@
         <v>6</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>10</v>
@@ -3455,7 +3470,7 @@
       </c>
       <c r="G128" s="2"/>
       <c r="H128" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I128" s="2"/>
     </row>
@@ -3464,7 +3479,7 @@
         <v>7</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>10</v>
@@ -3476,7 +3491,7 @@
       </c>
       <c r="G129" s="2"/>
       <c r="H129" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I129" s="2"/>
     </row>
@@ -3523,7 +3538,7 @@
         <v>10</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>14</v>
@@ -3540,10 +3555,10 @@
         <v>11</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="5"/>
@@ -3551,27 +3566,31 @@
       <c r="G133" s="2"/>
       <c r="H133" s="6"/>
       <c r="I133" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="7" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
+    <mergeCell ref="A2:I3"/>
+    <mergeCell ref="A12:I13"/>
+    <mergeCell ref="A24:I25"/>
+    <mergeCell ref="A84:I85"/>
+    <mergeCell ref="A97:I98"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="A32:A41"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A121:E121"/>
-    <mergeCell ref="E37:I37"/>
     <mergeCell ref="A42:A52"/>
-    <mergeCell ref="E47:I47"/>
     <mergeCell ref="A71:I72"/>
     <mergeCell ref="E55:I55"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="A53:A59"/>
     <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="A2:I3"/>
-    <mergeCell ref="A12:I13"/>
-    <mergeCell ref="A24:I25"/>
-    <mergeCell ref="A84:I85"/>
-    <mergeCell ref="A97:I98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3598,22 +3617,22 @@
   <sheetData>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
         <v>110</v>
       </c>
-      <c r="C6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>113</v>
-      </c>
-      <c r="E6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continue to update Order function
</commit_message>
<xml_diff>
--- a/Database ToCoShop.xlsx
+++ b/Database ToCoShop.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="136">
   <si>
     <t>No.</t>
   </si>
@@ -396,13 +396,40 @@
   </si>
   <si>
     <t>ngay chuyen hang co the la ngay mai hay phai la hom nay hoac qua khu</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>làm rõ tài liệu database- như file excel</t>
+  </si>
+  <si>
+    <t>làm các mô tả theo yêu cầu trong tài liệu mẫu</t>
+  </si>
+  <si>
+    <t>mô tả sản phẩm gồm những chức năng gì- chia theo nhóm- nhóm employees gồmn những chức năng gì</t>
+  </si>
+  <si>
+    <t>Mục tiêu dự án- ko chỉ cho develop hiểu mà còn cho team hiểu, người quản lý dự án hiểu</t>
+  </si>
+  <si>
+    <t>Ma don hang: o-ngay thang nam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o2210-số thự tự </t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>attributes: { sizes: [ {id:1, size: "XL", price: 10, stock: 10, discount: 5} ] }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +522,12 @@
       <color rgb="FF232629"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -746,7 +779,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1038,6 +1071,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1345,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I146"/>
+  <dimension ref="A2:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2445,27 +2482,27 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="121"/>
       <c r="B62" s="10" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
-      <c r="F62" s="10"/>
+      <c r="F62" s="14"/>
       <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
+      <c r="H62" s="14"/>
       <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="121"/>
       <c r="B63" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D63" s="10"/>
+      <c r="D63" s="12"/>
       <c r="E63" s="13"/>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
@@ -2475,10 +2512,10 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="121"/>
       <c r="B64" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="13"/>
@@ -2488,205 +2525,200 @@
       <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="113">
+      <c r="A65" s="121"/>
+      <c r="B65" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="10"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="113">
         <v>9</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B66" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="15"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="114"/>
-      <c r="B66" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" s="12"/>
+      <c r="D66" s="15"/>
       <c r="E66" s="13"/>
-      <c r="F66" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G66" s="10"/>
-      <c r="H66" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I66" s="10"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="114"/>
       <c r="B67" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="12">
-        <v>50</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D67" s="12"/>
       <c r="E67" s="13"/>
-      <c r="F67" s="14"/>
+      <c r="F67" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G67" s="10"/>
       <c r="H67" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I67" s="10"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="114"/>
+      <c r="B68" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="12">
+        <v>50</v>
+      </c>
+      <c r="E68" s="13"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="I67" s="10"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="115"/>
-      <c r="B68" s="10" t="s">
+      <c r="I68" s="10"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="115"/>
+      <c r="B69" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="12">
+      <c r="C69" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="12">
         <v>500</v>
       </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="10"/>
-      <c r="I68" s="10"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="116" t="s">
+      <c r="E69" s="13"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="116"/>
-      <c r="C71" s="116"/>
-      <c r="D71" s="116"/>
-      <c r="E71" s="116"/>
-      <c r="F71" s="116"/>
-      <c r="G71" s="116"/>
-      <c r="H71" s="116"/>
-      <c r="I71" s="116"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="117"/>
-      <c r="B72" s="117"/>
-      <c r="C72" s="117"/>
-      <c r="D72" s="117"/>
-      <c r="E72" s="117"/>
-      <c r="F72" s="117"/>
-      <c r="G72" s="117"/>
-      <c r="H72" s="117"/>
-      <c r="I72" s="117"/>
+      <c r="B72" s="116"/>
+      <c r="C72" s="116"/>
+      <c r="D72" s="116"/>
+      <c r="E72" s="116"/>
+      <c r="F72" s="116"/>
+      <c r="G72" s="116"/>
+      <c r="H72" s="116"/>
+      <c r="I72" s="116"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="45" t="s">
+      <c r="A73" s="117"/>
+      <c r="B73" s="117"/>
+      <c r="C73" s="117"/>
+      <c r="D73" s="117"/>
+      <c r="E73" s="117"/>
+      <c r="F73" s="117"/>
+      <c r="G73" s="117"/>
+      <c r="H73" s="117"/>
+      <c r="I73" s="117"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="45" t="s">
+      <c r="B74" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="45" t="s">
+      <c r="C74" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D73" s="45" t="s">
+      <c r="D74" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E73" s="45" t="s">
+      <c r="E74" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F73" s="45" t="s">
+      <c r="F74" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G73" s="45" t="s">
+      <c r="G74" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H73" s="45" t="s">
+      <c r="H74" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I73" s="45" t="s">
+      <c r="I74" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="46">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="46">
         <v>1</v>
       </c>
-      <c r="B74" s="46" t="s">
+      <c r="B75" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="47" t="s">
+      <c r="C75" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D74" s="48"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="46" t="s">
+      <c r="D75" s="48"/>
+      <c r="E75" s="49"/>
+      <c r="F75" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G74" s="46"/>
-      <c r="H74" s="46" t="s">
+      <c r="G75" s="46"/>
+      <c r="H75" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I74" s="46"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="50">
-        <f>A74+1</f>
-        <v>2</v>
-      </c>
-      <c r="B75" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="53">
-        <v>50</v>
-      </c>
-      <c r="E75" s="54"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="55"/>
-      <c r="H75" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="I75" s="55"/>
+      <c r="I75" s="46"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="50">
         <f>A75+1</f>
-        <v>3</v>
-      </c>
-      <c r="B76" s="64" t="s">
-        <v>101</v>
-      </c>
-      <c r="C76" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="D76" s="53"/>
+        <v>2</v>
+      </c>
+      <c r="B76" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="53">
+        <v>50</v>
+      </c>
       <c r="E76" s="54"/>
       <c r="F76" s="55"/>
       <c r="G76" s="55"/>
-      <c r="H76" s="50"/>
+      <c r="H76" s="50" t="s">
+        <v>15</v>
+      </c>
       <c r="I76" s="55"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="105">
-        <f t="shared" ref="A77:A80" si="2">A76+1</f>
-        <v>4</v>
-      </c>
-      <c r="B77" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C77" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="53">
-        <v>50</v>
-      </c>
+      <c r="A77" s="50">
+        <f>A76+1</f>
+        <v>3</v>
+      </c>
+      <c r="B77" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="C77" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77" s="53"/>
       <c r="E77" s="54"/>
       <c r="F77" s="55"/>
       <c r="G77" s="55"/>
@@ -2694,12 +2726,12 @@
       <c r="I77" s="55"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="50">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B78" s="106" t="s">
-        <v>103</v>
+      <c r="A78" s="105">
+        <f t="shared" ref="A78:A81" si="2">A77+1</f>
+        <v>4</v>
+      </c>
+      <c r="B78" s="51" t="s">
+        <v>102</v>
       </c>
       <c r="C78" s="52" t="s">
         <v>14</v>
@@ -2707,154 +2739,155 @@
       <c r="D78" s="53">
         <v>50</v>
       </c>
-      <c r="E78" s="56"/>
-      <c r="F78" s="50"/>
-      <c r="G78" s="50"/>
+      <c r="E78" s="54"/>
+      <c r="F78" s="55"/>
+      <c r="G78" s="55"/>
       <c r="H78" s="50"/>
-      <c r="I78" s="50"/>
+      <c r="I78" s="55"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="50">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B79" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="C79" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" s="59">
+        <v>5</v>
+      </c>
+      <c r="B79" s="106" t="s">
+        <v>103</v>
+      </c>
+      <c r="C79" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="53">
         <v>50</v>
       </c>
-      <c r="E79" s="60"/>
-      <c r="F79" s="61"/>
-      <c r="G79" s="61"/>
-      <c r="H79" s="61"/>
-      <c r="I79" s="61"/>
+      <c r="E79" s="56"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="50"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="50">
         <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B80" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="59">
+        <v>50</v>
+      </c>
+      <c r="E80" s="60"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
+      <c r="H80" s="61"/>
+      <c r="I80" s="61"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="50">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B80" s="50" t="s">
+      <c r="B81" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C80" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="63">
+      <c r="C81" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="63">
         <v>200</v>
       </c>
-      <c r="E80" s="56" t="s">
+      <c r="E81" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="F80" s="50"/>
-      <c r="G80" s="50"/>
-      <c r="H80" s="50"/>
-      <c r="I80" s="50"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="122" t="s">
+      <c r="F81" s="50"/>
+      <c r="G81" s="50"/>
+      <c r="H81" s="50"/>
+      <c r="I81" s="50"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="122" t="s">
         <v>65</v>
       </c>
-      <c r="B84" s="122"/>
-      <c r="C84" s="122"/>
-      <c r="D84" s="122"/>
-      <c r="E84" s="122"/>
-      <c r="F84" s="122"/>
-      <c r="G84" s="122"/>
-      <c r="H84" s="122"/>
-      <c r="I84" s="122"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="125"/>
-      <c r="B85" s="125"/>
-      <c r="C85" s="125"/>
-      <c r="D85" s="125"/>
-      <c r="E85" s="125"/>
-      <c r="F85" s="125"/>
-      <c r="G85" s="125"/>
-      <c r="H85" s="125"/>
-      <c r="I85" s="125"/>
+      <c r="B85" s="122"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
+      <c r="E85" s="122"/>
+      <c r="F85" s="122"/>
+      <c r="G85" s="122"/>
+      <c r="H85" s="122"/>
+      <c r="I85" s="122"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="39" t="s">
+      <c r="A86" s="125"/>
+      <c r="B86" s="125"/>
+      <c r="C86" s="125"/>
+      <c r="D86" s="125"/>
+      <c r="E86" s="125"/>
+      <c r="F86" s="125"/>
+      <c r="G86" s="125"/>
+      <c r="H86" s="125"/>
+      <c r="I86" s="125"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="39" t="s">
+      <c r="B87" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C86" s="39" t="s">
+      <c r="C87" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D86" s="39" t="s">
+      <c r="D87" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E86" s="39" t="s">
+      <c r="E87" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F86" s="39" t="s">
+      <c r="F87" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G86" s="39" t="s">
+      <c r="G87" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H86" s="39" t="s">
+      <c r="H87" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I86" s="39" t="s">
+      <c r="I87" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="40">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="40">
         <v>1</v>
       </c>
-      <c r="B87" s="40" t="s">
+      <c r="B88" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C87" s="41" t="s">
+      <c r="C88" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D87" s="42"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="40" t="s">
+      <c r="D88" s="42"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G87" s="40"/>
-      <c r="H87" s="40" t="s">
+      <c r="G88" s="40"/>
+      <c r="H88" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I87" s="44"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="36">
-        <f>A87+1</f>
-        <v>2</v>
-      </c>
-      <c r="B88" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C88" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" s="37">
-        <v>50</v>
-      </c>
-      <c r="E88" s="38"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
-      <c r="I88" s="36"/>
+      <c r="I88" s="44"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="36">
-        <f t="shared" ref="A89:A91" si="3">A88+1</f>
-        <v>3</v>
+        <f>A88+1</f>
+        <v>2</v>
       </c>
       <c r="B89" s="36" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="C89" s="35" t="s">
         <v>14</v>
@@ -2865,323 +2898,323 @@
       <c r="E89" s="38"/>
       <c r="F89" s="36"/>
       <c r="G89" s="36"/>
-      <c r="H89" s="36"/>
       <c r="I89" s="36"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="36">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="B90" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C90" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" s="28">
+        <f t="shared" ref="A90:A92" si="3">A89+1</f>
+        <v>3</v>
+      </c>
+      <c r="B90" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="37">
         <v>50</v>
       </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H90" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="I90" s="24"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="36"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="36"/>
+      <c r="I90" s="36"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="36">
         <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C91" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="28">
+        <v>50</v>
+      </c>
+      <c r="E91" s="8"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H91" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I91" s="24"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="36">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B91" s="36" t="s">
+      <c r="B92" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C91" s="35" t="s">
+      <c r="C92" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="D91" s="37"/>
-      <c r="E91" s="38"/>
-      <c r="F91" s="36"/>
-      <c r="G91" s="24" t="s">
+      <c r="D92" s="37"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="36"/>
+      <c r="G92" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="H91" s="24" t="s">
+      <c r="H92" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="I91" s="36"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="67"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="122" t="s">
+      <c r="I92" s="36"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="67"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="B97" s="122"/>
-      <c r="C97" s="122"/>
-      <c r="D97" s="122"/>
-      <c r="E97" s="122"/>
-      <c r="F97" s="122"/>
-      <c r="G97" s="122"/>
-      <c r="H97" s="122"/>
-      <c r="I97" s="122"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="125"/>
-      <c r="B98" s="125"/>
-      <c r="C98" s="125"/>
-      <c r="D98" s="125"/>
-      <c r="E98" s="125"/>
-      <c r="F98" s="125"/>
-      <c r="G98" s="125"/>
-      <c r="H98" s="125"/>
-      <c r="I98" s="125"/>
+      <c r="B98" s="122"/>
+      <c r="C98" s="122"/>
+      <c r="D98" s="122"/>
+      <c r="E98" s="122"/>
+      <c r="F98" s="122"/>
+      <c r="G98" s="122"/>
+      <c r="H98" s="122"/>
+      <c r="I98" s="122"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="39" t="s">
+      <c r="A99" s="125"/>
+      <c r="B99" s="125"/>
+      <c r="C99" s="125"/>
+      <c r="D99" s="125"/>
+      <c r="E99" s="125"/>
+      <c r="F99" s="125"/>
+      <c r="G99" s="125"/>
+      <c r="H99" s="125"/>
+      <c r="I99" s="125"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="39" t="s">
+      <c r="B100" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="39" t="s">
+      <c r="C100" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D99" s="39" t="s">
+      <c r="D100" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E99" s="39" t="s">
+      <c r="E100" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F99" s="39" t="s">
+      <c r="F100" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G99" s="39" t="s">
+      <c r="G100" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H99" s="39" t="s">
+      <c r="H100" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I99" s="39" t="s">
+      <c r="I100" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="40">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="40">
         <v>1</v>
       </c>
-      <c r="B100" s="40" t="s">
+      <c r="B101" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="41" t="s">
+      <c r="C101" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D100" s="42"/>
-      <c r="E100" s="43"/>
-      <c r="F100" s="40" t="s">
+      <c r="D101" s="42"/>
+      <c r="E101" s="43"/>
+      <c r="F101" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G100" s="40"/>
-      <c r="H100" s="40" t="s">
+      <c r="G101" s="40"/>
+      <c r="H101" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I100" s="44"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="36">
-        <f>A100+1</f>
-        <v>2</v>
-      </c>
-      <c r="B101" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="C101" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D101" s="37">
-        <v>50</v>
-      </c>
-      <c r="E101" s="38"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="68"/>
-      <c r="I101" s="36"/>
+      <c r="I101" s="44"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="36">
-        <f t="shared" ref="A102:A104" si="4">A101+1</f>
-        <v>3</v>
+        <f>A101+1</f>
+        <v>2</v>
       </c>
       <c r="B102" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C102" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D102" s="37">
-        <v>500</v>
-      </c>
-      <c r="E102" s="38" t="s">
-        <v>17</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E102" s="38"/>
       <c r="F102" s="36"/>
       <c r="G102" s="36"/>
-      <c r="H102" s="36"/>
+      <c r="H102" s="68"/>
       <c r="I102" s="36"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="36">
+        <f t="shared" ref="A103:A105" si="4">A102+1</f>
+        <v>3</v>
+      </c>
+      <c r="B103" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C103" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" s="37">
+        <v>500</v>
+      </c>
+      <c r="E103" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F103" s="36"/>
+      <c r="G103" s="36"/>
+      <c r="H103" s="36"/>
+      <c r="I103" s="36"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="36">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B103" s="27" t="s">
+      <c r="B104" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C103" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" s="28" t="s">
+      <c r="C104" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E103" s="8"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="24"/>
-      <c r="H103" s="24"/>
-      <c r="I103" s="24"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="69">
+      <c r="E104" s="8"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="24"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="69">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B104" s="69" t="s">
+      <c r="B105" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="C104" s="70" t="s">
+      <c r="C105" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="D104" s="71"/>
-      <c r="E104" s="72"/>
-      <c r="F104" s="69"/>
-      <c r="G104" s="73"/>
-      <c r="H104" s="73" t="s">
+      <c r="D105" s="71"/>
+      <c r="E105" s="72"/>
+      <c r="F105" s="69"/>
+      <c r="G105" s="73"/>
+      <c r="H105" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="I104" s="69"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="74">
+      <c r="I105" s="69"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="74">
         <v>6</v>
       </c>
-      <c r="B105" s="74" t="s">
+      <c r="B106" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C105" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D105" s="74"/>
-      <c r="E105" s="74"/>
-      <c r="F105" s="74"/>
-      <c r="G105" s="75" t="s">
+      <c r="C106" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" s="74"/>
+      <c r="E106" s="74"/>
+      <c r="F106" s="74"/>
+      <c r="G106" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="H105" s="75" t="s">
+      <c r="H106" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="I105" s="74"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="110" t="s">
+      <c r="I106" s="74"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="110" t="s">
         <v>80</v>
       </c>
-      <c r="B109" s="111"/>
-      <c r="C109" s="111"/>
-      <c r="D109" s="111"/>
-      <c r="E109" s="111"/>
-      <c r="F109" s="77"/>
-      <c r="G109" s="77"/>
-      <c r="H109" s="77"/>
-      <c r="I109" s="77"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="78" t="s">
+      <c r="B110" s="111"/>
+      <c r="C110" s="111"/>
+      <c r="D110" s="111"/>
+      <c r="E110" s="111"/>
+      <c r="F110" s="77"/>
+      <c r="G110" s="77"/>
+      <c r="H110" s="77"/>
+      <c r="I110" s="77"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B110" s="78" t="s">
+      <c r="B111" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C110" s="78" t="s">
+      <c r="C111" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D110" s="78" t="s">
+      <c r="D111" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E110" s="78" t="s">
+      <c r="E111" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F110" s="78" t="s">
+      <c r="F111" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="G110" s="78" t="s">
+      <c r="G111" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="H110" s="78" t="s">
+      <c r="H111" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="I110" s="78" t="s">
+      <c r="I111" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="79">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="79">
         <v>1</v>
       </c>
-      <c r="B111" s="79" t="s">
+      <c r="B112" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="80" t="s">
+      <c r="C112" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D111" s="81">
+      <c r="D112" s="81">
         <v>50</v>
       </c>
-      <c r="E111" s="82"/>
-      <c r="F111" s="79" t="s">
+      <c r="E112" s="82"/>
+      <c r="F112" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G111" s="79"/>
-      <c r="H111" s="79"/>
-      <c r="I111" s="79"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="83">
-        <v>2</v>
-      </c>
-      <c r="B112" s="83" t="s">
-        <v>54</v>
-      </c>
-      <c r="C112" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D112" s="85">
-        <v>50</v>
-      </c>
-      <c r="E112" s="86"/>
-      <c r="F112" s="83"/>
-      <c r="G112" s="83"/>
-      <c r="H112" s="83"/>
-      <c r="I112" s="83"/>
+      <c r="G112" s="79"/>
+      <c r="H112" s="79"/>
+      <c r="I112" s="79"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B113" s="83" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C113" s="84" t="s">
         <v>14</v>
@@ -3197,10 +3230,10 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B114" s="83" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C114" s="84" t="s">
         <v>14</v>
@@ -3208,9 +3241,7 @@
       <c r="D114" s="85">
         <v>50</v>
       </c>
-      <c r="E114" s="86" t="s">
-        <v>17</v>
-      </c>
+      <c r="E114" s="86"/>
       <c r="F114" s="83"/>
       <c r="G114" s="83"/>
       <c r="H114" s="83"/>
@@ -3218,75 +3249,85 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B115" s="83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C115" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D115" s="85">
-        <v>500</v>
-      </c>
-      <c r="E115" s="86"/>
+        <v>50</v>
+      </c>
+      <c r="E115" s="86" t="s">
+        <v>17</v>
+      </c>
       <c r="F115" s="83"/>
       <c r="G115" s="83"/>
-      <c r="H115" s="68" t="s">
-        <v>68</v>
-      </c>
+      <c r="H115" s="83"/>
       <c r="I115" s="83"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B116" s="83" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C116" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D116" s="85">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E116" s="86"/>
       <c r="F116" s="83"/>
       <c r="G116" s="83"/>
-      <c r="H116" s="83" t="s">
+      <c r="H116" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="I116" s="83"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" s="83">
+        <v>6</v>
+      </c>
+      <c r="B117" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="85">
+        <v>50</v>
+      </c>
+      <c r="E117" s="86"/>
+      <c r="F117" s="83"/>
+      <c r="G117" s="83"/>
+      <c r="H117" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="I116" s="83"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="98">
+      <c r="I117" s="83"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" s="98">
         <v>7</v>
       </c>
-      <c r="B117" s="98" t="s">
+      <c r="B118" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="C117" s="99" t="s">
+      <c r="C118" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="D117" s="100"/>
-      <c r="E117" s="101" t="s">
+      <c r="D118" s="100"/>
+      <c r="E118" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F117" s="98"/>
-      <c r="G117" s="98"/>
-      <c r="H117" s="98"/>
-      <c r="I117" s="98"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="94"/>
-      <c r="B118" s="94"/>
-      <c r="C118" s="95"/>
-      <c r="D118" s="96"/>
-      <c r="E118" s="97"/>
-      <c r="F118" s="94"/>
-      <c r="G118" s="94"/>
-      <c r="H118" s="94"/>
-      <c r="I118" s="94"/>
+      <c r="F118" s="98"/>
+      <c r="G118" s="98"/>
+      <c r="H118" s="98"/>
+      <c r="I118" s="98"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="94"/>
@@ -3300,125 +3341,115 @@
       <c r="I119" s="94"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="102"/>
-      <c r="B120" s="102"/>
-      <c r="C120" s="102"/>
-      <c r="D120" s="102"/>
-      <c r="E120" s="102"/>
-      <c r="F120" s="102"/>
-      <c r="G120" s="102"/>
-      <c r="H120" s="102"/>
-      <c r="I120" s="102"/>
+      <c r="A120" s="94"/>
+      <c r="B120" s="94"/>
+      <c r="C120" s="95"/>
+      <c r="D120" s="96"/>
+      <c r="E120" s="97"/>
+      <c r="F120" s="94"/>
+      <c r="G120" s="94"/>
+      <c r="H120" s="94"/>
+      <c r="I120" s="94"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="112" t="s">
+      <c r="A121" s="102"/>
+      <c r="B121" s="102"/>
+      <c r="C121" s="102"/>
+      <c r="D121" s="102"/>
+      <c r="E121" s="102"/>
+      <c r="F121" s="102"/>
+      <c r="G121" s="102"/>
+      <c r="H121" s="102"/>
+      <c r="I121" s="102"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="B121" s="111"/>
-      <c r="C121" s="111"/>
-      <c r="D121" s="111"/>
-      <c r="E121" s="111"/>
-      <c r="F121" s="87"/>
-      <c r="G121" s="87"/>
-      <c r="H121" s="87"/>
-      <c r="I121" s="87"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="88" t="s">
+      <c r="B122" s="111"/>
+      <c r="C122" s="111"/>
+      <c r="D122" s="111"/>
+      <c r="E122" s="111"/>
+      <c r="F122" s="87"/>
+      <c r="G122" s="87"/>
+      <c r="H122" s="87"/>
+      <c r="I122" s="87"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B122" s="88" t="s">
+      <c r="B123" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C122" s="88" t="s">
+      <c r="C123" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D122" s="88" t="s">
+      <c r="D123" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E122" s="88" t="s">
+      <c r="E123" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F122" s="88" t="s">
+      <c r="F123" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G122" s="88" t="s">
+      <c r="G123" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H122" s="88" t="s">
+      <c r="H123" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I122" s="88" t="s">
+      <c r="I123" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="1">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
         <v>1</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C123" s="89" t="s">
+      <c r="C124" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D123" s="90"/>
-      <c r="E123" s="91"/>
-      <c r="F123" s="1" t="s">
+      <c r="D124" s="90"/>
+      <c r="E124" s="91"/>
+      <c r="F124" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1" t="s">
+      <c r="G124" s="1"/>
+      <c r="H124" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I123" s="1"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="2">
-        <v>2</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D124" s="92">
-        <v>50</v>
-      </c>
-      <c r="E124" s="93"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="6"/>
-      <c r="H124" s="6"/>
-      <c r="I124" s="6"/>
+      <c r="I124" s="1"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D125" s="4"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="2"/>
-      <c r="G125" s="2">
-        <v>0</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I125" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D125" s="92">
+        <v>50</v>
+      </c>
+      <c r="E125" s="93"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>42</v>
@@ -3430,16 +3461,16 @@
         <v>0</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>42</v>
@@ -3450,36 +3481,36 @@
       <c r="G127" s="2">
         <v>0</v>
       </c>
-      <c r="H127" s="2"/>
+      <c r="H127" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="5"/>
-      <c r="F128" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G128" s="2"/>
-      <c r="H128" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2">
+        <v>0</v>
+      </c>
+      <c r="H128" s="2"/>
       <c r="I128" s="2"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>10</v>
@@ -3491,86 +3522,160 @@
       </c>
       <c r="G129" s="2"/>
       <c r="H129" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I129" s="2"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
+        <v>7</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D130" s="4"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G130" s="2"/>
+      <c r="H130" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I130" s="2"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
         <v>8</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C130" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D130" s="4" t="s">
+      <c r="C131" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E130" s="5"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="2"/>
-      <c r="H130" s="6"/>
-      <c r="I130" s="2"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A131" s="103">
-        <v>9</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D131" s="4"/>
       <c r="E131" s="5"/>
       <c r="F131" s="6"/>
       <c r="G131" s="2"/>
       <c r="H131" s="6"/>
-      <c r="I131" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="I131" s="2"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="103">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="5"/>
       <c r="F132" s="6"/>
       <c r="G132" s="2"/>
       <c r="H132" s="6"/>
-      <c r="I132" s="2"/>
+      <c r="I132" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="2">
-        <v>11</v>
+      <c r="A133" s="103">
+        <v>10</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="5"/>
       <c r="F133" s="6"/>
       <c r="G133" s="2"/>
       <c r="H133" s="6"/>
-      <c r="I133" s="2" t="s">
+      <c r="I133" s="2"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>11</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D134" s="4"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="6"/>
+      <c r="I134" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B146" s="7" t="s">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="7">
+        <v>12</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C136" s="127"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C137" s="127"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C138" s="127"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B140" s="126" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B142" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B143" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B144" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B145" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B150" s="7" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3579,18 +3684,18 @@
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A12:I13"/>
     <mergeCell ref="A24:I25"/>
-    <mergeCell ref="A84:I85"/>
-    <mergeCell ref="A97:I98"/>
+    <mergeCell ref="A85:I86"/>
+    <mergeCell ref="A98:I99"/>
     <mergeCell ref="F47:I47"/>
     <mergeCell ref="A32:A41"/>
-    <mergeCell ref="A109:E109"/>
-    <mergeCell ref="A121:E121"/>
+    <mergeCell ref="A110:E110"/>
+    <mergeCell ref="A122:E122"/>
     <mergeCell ref="A42:A52"/>
-    <mergeCell ref="A71:I72"/>
+    <mergeCell ref="A72:I73"/>
     <mergeCell ref="E55:I55"/>
-    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A60:A65"/>
     <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A66:A69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
continue to set up order function
</commit_message>
<xml_diff>
--- a/Database ToCoShop.xlsx
+++ b/Database ToCoShop.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="137">
   <si>
     <t>No.</t>
   </si>
@@ -419,10 +419,13 @@
     <t xml:space="preserve">o2210-số thự tự </t>
   </si>
   <si>
-    <t>Attribute</t>
-  </si>
-  <si>
     <t>attributes: { sizes: [ {id:1, size: "XL", price: 10, stock: 10, discount: 5} ] }</t>
+  </si>
+  <si>
+    <t>OrderCode</t>
+  </si>
+  <si>
+    <t>AUTO</t>
   </si>
 </sst>
 </file>
@@ -779,7 +782,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1026,6 +1029,43 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1033,47 +1073,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1382,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I150"/>
+  <dimension ref="A2:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136:C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1403,28 +1410,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
     </row>
     <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="123"/>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
+      <c r="A3" s="113"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
     </row>
     <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -1565,28 +1572,28 @@
       <c r="I9" s="24"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="114"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="117"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="117"/>
+      <c r="A13" s="115"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
@@ -1763,28 +1770,28 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="124"/>
-      <c r="C24" s="124"/>
-      <c r="D24" s="124"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="124"/>
-      <c r="I24" s="124"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="116"/>
     </row>
     <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="124"/>
-      <c r="B25" s="124"/>
-      <c r="C25" s="124"/>
-      <c r="D25" s="124"/>
-      <c r="E25" s="124"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="124"/>
-      <c r="I25" s="124"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="116"/>
+      <c r="I25" s="116"/>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -1836,55 +1843,57 @@
       </c>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <f>A27+1</f>
         <v>2</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="D28" s="12">
+        <v>50</v>
+      </c>
       <c r="E28" s="13"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
-        <v>32</v>
-      </c>
+      <c r="G28" s="10"/>
       <c r="H28" s="10" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
+        <f t="shared" ref="A29:A32" si="2">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>114</v>
+        <v>30</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="12"/>
-      <c r="E29" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="G29" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="H29" s="10" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>31</v>
@@ -1896,71 +1905,75 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10" t="s">
+      <c r="C32" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="113">
-        <v>5</v>
-      </c>
-      <c r="B32" s="14" t="s">
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="120">
+        <v>7</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="114"/>
-      <c r="B33" s="10" t="s">
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="121"/>
+      <c r="B34" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="12">
-        <v>50</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="I33" s="10"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="114"/>
-      <c r="B34" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>14</v>
@@ -1968,9 +1981,7 @@
       <c r="D34" s="12">
         <v>50</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="E34" s="13"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="14" t="s">
@@ -1979,9 +1990,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="114"/>
+      <c r="A35" s="121"/>
       <c r="B35" s="10" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>14</v>
@@ -1989,18 +2000,20 @@
       <c r="D35" s="12">
         <v>50</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="F35" s="10"/>
-      <c r="G35" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="114"/>
+      <c r="A36" s="121"/>
       <c r="B36" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>14</v>
@@ -2016,46 +2029,46 @@
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A37" s="114"/>
-      <c r="B37" s="29" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="121"/>
+      <c r="B37" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="12">
+        <v>50</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A38" s="121"/>
+      <c r="B38" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C38" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="31"/>
-      <c r="E37" s="107" t="s">
+      <c r="D38" s="31"/>
+      <c r="E38" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="108"/>
-      <c r="G37" s="108"/>
-      <c r="H37" s="108"/>
-      <c r="I37" s="109"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="114"/>
-      <c r="B38" s="32" t="s">
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="108"/>
+      <c r="I38" s="109"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="121"/>
+      <c r="B39" s="32" t="s">
         <v>51</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="34">
-        <v>50</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="114"/>
-      <c r="B39" s="32" t="s">
-        <v>119</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>14</v>
@@ -2072,9 +2085,9 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="114"/>
+      <c r="A40" s="121"/>
       <c r="B40" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>14</v>
@@ -2091,85 +2104,85 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="115"/>
+      <c r="A41" s="121"/>
       <c r="B41" s="32" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="34">
-        <v>500</v>
-      </c>
-      <c r="E41" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="F41" s="10"/>
-      <c r="G41" s="10" t="s">
-        <v>121</v>
-      </c>
+      <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="113">
-        <v>6</v>
-      </c>
-      <c r="B42" s="14" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="122"/>
+      <c r="B42" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="34">
+        <v>500</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="120">
+        <v>8</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="15"/>
-      <c r="E42" s="13" t="s">
+      <c r="D43" s="15"/>
+      <c r="E43" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="114"/>
-      <c r="B43" s="10" t="s">
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="121"/>
+      <c r="B44" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C44" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="14" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="14" t="s">
+      <c r="G44" s="10"/>
+      <c r="H44" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I43" s="10"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="114"/>
-      <c r="B44" s="10" t="s">
+      <c r="I44" s="10"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="121"/>
+      <c r="B45" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="12">
-        <v>50</v>
-      </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="114"/>
-      <c r="B45" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>14</v>
@@ -2186,9 +2199,9 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="114"/>
+      <c r="A46" s="121"/>
       <c r="B46" s="10" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>14</v>
@@ -2198,54 +2211,54 @@
       </c>
       <c r="E46" s="13"/>
       <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="14" t="s">
+      <c r="G46" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="121"/>
+      <c r="B47" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="12">
+        <v>50</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I46" s="10"/>
-    </row>
-    <row r="47" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A47" s="114"/>
-      <c r="B47" s="29" t="s">
+      <c r="I47" s="10"/>
+    </row>
+    <row r="48" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A48" s="121"/>
+      <c r="B48" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C48" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="31"/>
-      <c r="E47" s="107" t="s">
+      <c r="D48" s="31"/>
+      <c r="E48" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="119" t="s">
+      <c r="F48" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="G47" s="119"/>
-      <c r="H47" s="119"/>
-      <c r="I47" s="120"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="114"/>
-      <c r="B48" s="32" t="s">
+      <c r="G48" s="118"/>
+      <c r="H48" s="118"/>
+      <c r="I48" s="119"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="121"/>
+      <c r="B49" s="32" t="s">
         <v>51</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="34">
-        <v>50</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="114"/>
-      <c r="B49" s="32" t="s">
-        <v>119</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>14</v>
@@ -2262,9 +2275,9 @@
       <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="114"/>
+      <c r="A50" s="121"/>
       <c r="B50" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>14</v>
@@ -2281,243 +2294,247 @@
       <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="114"/>
+      <c r="A51" s="121"/>
       <c r="B51" s="32" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="34">
-        <v>500</v>
-      </c>
-      <c r="E51" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="F51" s="10"/>
-      <c r="G51" s="10" t="s">
-        <v>121</v>
-      </c>
+      <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="115"/>
-      <c r="B52" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="12">
-        <v>200</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A52" s="121"/>
+      <c r="B52" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="34">
+        <v>500</v>
+      </c>
+      <c r="E52" s="13"/>
       <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
+      <c r="G52" s="10" t="s">
+        <v>121</v>
+      </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
     </row>
-    <row r="53" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="113">
-        <v>7</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" s="15"/>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="122"/>
+      <c r="B53" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="12">
+        <v>200</v>
+      </c>
       <c r="E53" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="114"/>
-      <c r="B54" s="10" t="s">
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="120">
+        <v>9</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" s="15"/>
+      <c r="E54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="121"/>
+      <c r="B55" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10" t="s">
+      <c r="C55" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I54" s="10"/>
-    </row>
-    <row r="55" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A55" s="114"/>
-      <c r="B55" s="29" t="s">
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A56" s="121"/>
+      <c r="B56" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C56" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D55" s="31"/>
-      <c r="E55" s="118" t="s">
+      <c r="D56" s="31"/>
+      <c r="E56" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="F55" s="119"/>
-      <c r="G55" s="119"/>
-      <c r="H55" s="119"/>
-      <c r="I55" s="120"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="114"/>
-      <c r="B56" s="32" t="s">
+      <c r="F56" s="118"/>
+      <c r="G56" s="118"/>
+      <c r="H56" s="118"/>
+      <c r="I56" s="119"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="121"/>
+      <c r="B57" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="34"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="I56" s="10"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="114"/>
-      <c r="B57" s="32" t="s">
-        <v>95</v>
-      </c>
       <c r="C57" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="34">
-        <v>50</v>
-      </c>
+      <c r="D57" s="34"/>
       <c r="E57" s="13"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
+      <c r="H57" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="I57" s="10"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="114"/>
+      <c r="A58" s="121"/>
       <c r="B58" s="32" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D58" s="34"/>
+        <v>14</v>
+      </c>
+      <c r="D58" s="34">
+        <v>50</v>
+      </c>
       <c r="E58" s="13"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
-      <c r="H58" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="I58" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="115"/>
+      <c r="A59" s="121"/>
       <c r="B59" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="34">
-        <v>3</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D59" s="34"/>
       <c r="E59" s="13"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
-      <c r="H59" s="104" t="s">
+      <c r="H59" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="122"/>
+      <c r="B60" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="34">
+        <v>3</v>
+      </c>
+      <c r="E60" s="13"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="104" t="s">
         <v>98</v>
       </c>
-      <c r="I59" s="10"/>
-    </row>
-    <row r="60" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="121">
-        <v>8</v>
-      </c>
-      <c r="B60" s="14" t="s">
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="127">
+        <v>10</v>
+      </c>
+      <c r="B61" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="121"/>
-      <c r="B61" s="10" t="s">
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="127"/>
+      <c r="B62" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C62" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G61" s="10"/>
-      <c r="H61" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="I61" s="10"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="121"/>
-      <c r="B62" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>14</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
-      <c r="F62" s="14"/>
+      <c r="F62" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G62" s="10"/>
-      <c r="H62" s="14"/>
+      <c r="H62" s="14" t="s">
+        <v>124</v>
+      </c>
       <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="121"/>
+      <c r="A63" s="127"/>
       <c r="B63" s="10" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="13"/>
-      <c r="F63" s="10"/>
+      <c r="F63" s="14"/>
       <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
+      <c r="H63" s="14"/>
       <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="121"/>
+      <c r="A64" s="127"/>
       <c r="B64" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="10"/>
+      <c r="D64" s="12"/>
       <c r="E64" s="13"/>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
@@ -2525,12 +2542,12 @@
       <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="121"/>
+      <c r="A65" s="127"/>
       <c r="B65" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="13"/>
@@ -2540,205 +2557,200 @@
       <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="113">
-        <v>9</v>
-      </c>
-      <c r="B66" s="14" t="s">
+      <c r="A66" s="127"/>
+      <c r="B66" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="120">
+        <v>11</v>
+      </c>
+      <c r="B67" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C67" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="15"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="114"/>
-      <c r="B67" s="10" t="s">
+      <c r="D67" s="15"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="121"/>
+      <c r="B68" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C68" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D67" s="12"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="14" t="s">
+      <c r="D68" s="12"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G67" s="10"/>
-      <c r="H67" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I67" s="10"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="114"/>
-      <c r="B68" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="12">
-        <v>50</v>
-      </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="14"/>
       <c r="G68" s="10"/>
       <c r="H68" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I68" s="10"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="121"/>
+      <c r="B69" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="12">
+        <v>50</v>
+      </c>
+      <c r="E69" s="13"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="I68" s="10"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="115"/>
-      <c r="B69" s="10" t="s">
+      <c r="I69" s="10"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="122"/>
+      <c r="B70" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C69" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="12">
+      <c r="C70" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="12">
         <v>500</v>
       </c>
-      <c r="E69" s="13"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
-      <c r="H69" s="10"/>
-      <c r="I69" s="10"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="116" t="s">
+      <c r="E70" s="13"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="116"/>
-      <c r="C72" s="116"/>
-      <c r="D72" s="116"/>
-      <c r="E72" s="116"/>
-      <c r="F72" s="116"/>
-      <c r="G72" s="116"/>
-      <c r="H72" s="116"/>
-      <c r="I72" s="116"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="117"/>
-      <c r="B73" s="117"/>
-      <c r="C73" s="117"/>
-      <c r="D73" s="117"/>
-      <c r="E73" s="117"/>
-      <c r="F73" s="117"/>
-      <c r="G73" s="117"/>
-      <c r="H73" s="117"/>
-      <c r="I73" s="117"/>
+      <c r="B73" s="114"/>
+      <c r="C73" s="114"/>
+      <c r="D73" s="114"/>
+      <c r="E73" s="114"/>
+      <c r="F73" s="114"/>
+      <c r="G73" s="114"/>
+      <c r="H73" s="114"/>
+      <c r="I73" s="114"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="45" t="s">
+      <c r="A74" s="115"/>
+      <c r="B74" s="115"/>
+      <c r="C74" s="115"/>
+      <c r="D74" s="115"/>
+      <c r="E74" s="115"/>
+      <c r="F74" s="115"/>
+      <c r="G74" s="115"/>
+      <c r="H74" s="115"/>
+      <c r="I74" s="115"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="45" t="s">
+      <c r="B75" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="45" t="s">
+      <c r="C75" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="45" t="s">
+      <c r="D75" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E74" s="45" t="s">
+      <c r="E75" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F74" s="45" t="s">
+      <c r="F75" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G74" s="45" t="s">
+      <c r="G75" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H74" s="45" t="s">
+      <c r="H75" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I74" s="45" t="s">
+      <c r="I75" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="46">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="46">
         <v>1</v>
       </c>
-      <c r="B75" s="46" t="s">
+      <c r="B76" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="47" t="s">
+      <c r="C76" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="48"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="46" t="s">
+      <c r="D76" s="48"/>
+      <c r="E76" s="49"/>
+      <c r="F76" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G75" s="46"/>
-      <c r="H75" s="46" t="s">
+      <c r="G76" s="46"/>
+      <c r="H76" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I75" s="46"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="50">
-        <f>A75+1</f>
-        <v>2</v>
-      </c>
-      <c r="B76" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="53">
-        <v>50</v>
-      </c>
-      <c r="E76" s="54"/>
-      <c r="F76" s="55"/>
-      <c r="G76" s="55"/>
-      <c r="H76" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="I76" s="55"/>
+      <c r="I76" s="46"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="50">
         <f>A76+1</f>
-        <v>3</v>
-      </c>
-      <c r="B77" s="64" t="s">
-        <v>101</v>
-      </c>
-      <c r="C77" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="D77" s="53"/>
+        <v>2</v>
+      </c>
+      <c r="B77" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="53">
+        <v>50</v>
+      </c>
       <c r="E77" s="54"/>
       <c r="F77" s="55"/>
       <c r="G77" s="55"/>
-      <c r="H77" s="50"/>
+      <c r="H77" s="50" t="s">
+        <v>15</v>
+      </c>
       <c r="I77" s="55"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="105">
-        <f t="shared" ref="A78:A81" si="2">A77+1</f>
-        <v>4</v>
-      </c>
-      <c r="B78" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C78" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="53">
-        <v>50</v>
-      </c>
+      <c r="A78" s="50">
+        <f>A77+1</f>
+        <v>3</v>
+      </c>
+      <c r="B78" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D78" s="53"/>
       <c r="E78" s="54"/>
       <c r="F78" s="55"/>
       <c r="G78" s="55"/>
@@ -2746,12 +2758,12 @@
       <c r="I78" s="55"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="50">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B79" s="106" t="s">
-        <v>103</v>
+      <c r="A79" s="105">
+        <f t="shared" ref="A79:A82" si="3">A78+1</f>
+        <v>4</v>
+      </c>
+      <c r="B79" s="51" t="s">
+        <v>102</v>
       </c>
       <c r="C79" s="52" t="s">
         <v>14</v>
@@ -2759,154 +2771,155 @@
       <c r="D79" s="53">
         <v>50</v>
       </c>
-      <c r="E79" s="56"/>
-      <c r="F79" s="50"/>
-      <c r="G79" s="50"/>
+      <c r="E79" s="54"/>
+      <c r="F79" s="55"/>
+      <c r="G79" s="55"/>
       <c r="H79" s="50"/>
-      <c r="I79" s="50"/>
+      <c r="I79" s="55"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="50">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B80" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="C80" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="59">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B80" s="106" t="s">
+        <v>103</v>
+      </c>
+      <c r="C80" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="53">
         <v>50</v>
       </c>
-      <c r="E80" s="60"/>
-      <c r="F80" s="61"/>
-      <c r="G80" s="61"/>
-      <c r="H80" s="61"/>
-      <c r="I80" s="61"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="50"/>
+      <c r="G80" s="50"/>
+      <c r="H80" s="50"/>
+      <c r="I80" s="50"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B81" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="59">
+        <v>50</v>
+      </c>
+      <c r="E81" s="60"/>
+      <c r="F81" s="61"/>
+      <c r="G81" s="61"/>
+      <c r="H81" s="61"/>
+      <c r="I81" s="61"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="50">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B81" s="50" t="s">
+      <c r="B82" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C81" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" s="63">
+      <c r="C82" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="63">
         <v>200</v>
       </c>
-      <c r="E81" s="56" t="s">
+      <c r="E82" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="F81" s="50"/>
-      <c r="G81" s="50"/>
-      <c r="H81" s="50"/>
-      <c r="I81" s="50"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="122" t="s">
+      <c r="F82" s="50"/>
+      <c r="G82" s="50"/>
+      <c r="H82" s="50"/>
+      <c r="I82" s="50"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="B85" s="122"/>
-      <c r="C85" s="122"/>
-      <c r="D85" s="122"/>
-      <c r="E85" s="122"/>
-      <c r="F85" s="122"/>
-      <c r="G85" s="122"/>
-      <c r="H85" s="122"/>
-      <c r="I85" s="122"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="125"/>
-      <c r="B86" s="125"/>
-      <c r="C86" s="125"/>
-      <c r="D86" s="125"/>
-      <c r="E86" s="125"/>
-      <c r="F86" s="125"/>
-      <c r="G86" s="125"/>
-      <c r="H86" s="125"/>
-      <c r="I86" s="125"/>
+      <c r="B86" s="112"/>
+      <c r="C86" s="112"/>
+      <c r="D86" s="112"/>
+      <c r="E86" s="112"/>
+      <c r="F86" s="112"/>
+      <c r="G86" s="112"/>
+      <c r="H86" s="112"/>
+      <c r="I86" s="112"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="117"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="117"/>
+      <c r="D87" s="117"/>
+      <c r="E87" s="117"/>
+      <c r="F87" s="117"/>
+      <c r="G87" s="117"/>
+      <c r="H87" s="117"/>
+      <c r="I87" s="117"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B87" s="39" t="s">
+      <c r="B88" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C87" s="39" t="s">
+      <c r="C88" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D87" s="39" t="s">
+      <c r="D88" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E87" s="39" t="s">
+      <c r="E88" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F87" s="39" t="s">
+      <c r="F88" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G87" s="39" t="s">
+      <c r="G88" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H87" s="39" t="s">
+      <c r="H88" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I87" s="39" t="s">
+      <c r="I88" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="40">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="40">
         <v>1</v>
       </c>
-      <c r="B88" s="40" t="s">
+      <c r="B89" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="41" t="s">
+      <c r="C89" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D88" s="42"/>
-      <c r="E88" s="43"/>
-      <c r="F88" s="40" t="s">
+      <c r="D89" s="42"/>
+      <c r="E89" s="43"/>
+      <c r="F89" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G88" s="40"/>
-      <c r="H88" s="40" t="s">
+      <c r="G89" s="40"/>
+      <c r="H89" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I88" s="44"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="36">
-        <f>A88+1</f>
-        <v>2</v>
-      </c>
-      <c r="B89" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C89" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D89" s="37">
-        <v>50</v>
-      </c>
-      <c r="E89" s="38"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="36"/>
-      <c r="I89" s="36"/>
+      <c r="I89" s="44"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="36">
-        <f t="shared" ref="A90:A92" si="3">A89+1</f>
-        <v>3</v>
+        <f>A89+1</f>
+        <v>2</v>
       </c>
       <c r="B90" s="36" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="C90" s="35" t="s">
         <v>14</v>
@@ -2917,323 +2930,323 @@
       <c r="E90" s="38"/>
       <c r="F90" s="36"/>
       <c r="G90" s="36"/>
-      <c r="H90" s="36"/>
       <c r="I90" s="36"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="36">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="B91" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C91" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="28">
+        <f t="shared" ref="A91:A93" si="4">A90+1</f>
+        <v>3</v>
+      </c>
+      <c r="B91" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C91" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="37">
         <v>50</v>
       </c>
-      <c r="E91" s="8"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H91" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="I91" s="24"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="36"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="36"/>
+      <c r="I91" s="36"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="B92" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C92" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="28">
+        <v>50</v>
+      </c>
+      <c r="E92" s="8"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H92" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I92" s="24"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="36">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B92" s="36" t="s">
+      <c r="B93" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C92" s="35" t="s">
+      <c r="C93" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="D92" s="37"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="36"/>
-      <c r="G92" s="24" t="s">
+      <c r="D93" s="37"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="36"/>
+      <c r="G93" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="H92" s="24" t="s">
+      <c r="H93" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="I92" s="36"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="67"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="122" t="s">
+      <c r="I93" s="36"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="67"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="B98" s="122"/>
-      <c r="C98" s="122"/>
-      <c r="D98" s="122"/>
-      <c r="E98" s="122"/>
-      <c r="F98" s="122"/>
-      <c r="G98" s="122"/>
-      <c r="H98" s="122"/>
-      <c r="I98" s="122"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="125"/>
-      <c r="B99" s="125"/>
-      <c r="C99" s="125"/>
-      <c r="D99" s="125"/>
-      <c r="E99" s="125"/>
-      <c r="F99" s="125"/>
-      <c r="G99" s="125"/>
-      <c r="H99" s="125"/>
-      <c r="I99" s="125"/>
+      <c r="B99" s="112"/>
+      <c r="C99" s="112"/>
+      <c r="D99" s="112"/>
+      <c r="E99" s="112"/>
+      <c r="F99" s="112"/>
+      <c r="G99" s="112"/>
+      <c r="H99" s="112"/>
+      <c r="I99" s="112"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="39" t="s">
+      <c r="A100" s="117"/>
+      <c r="B100" s="117"/>
+      <c r="C100" s="117"/>
+      <c r="D100" s="117"/>
+      <c r="E100" s="117"/>
+      <c r="F100" s="117"/>
+      <c r="G100" s="117"/>
+      <c r="H100" s="117"/>
+      <c r="I100" s="117"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B100" s="39" t="s">
+      <c r="B101" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C100" s="39" t="s">
+      <c r="C101" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D100" s="39" t="s">
+      <c r="D101" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E100" s="39" t="s">
+      <c r="E101" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F100" s="39" t="s">
+      <c r="F101" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G100" s="39" t="s">
+      <c r="G101" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H100" s="39" t="s">
+      <c r="H101" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I100" s="39" t="s">
+      <c r="I101" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="40">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="40">
         <v>1</v>
       </c>
-      <c r="B101" s="40" t="s">
+      <c r="B102" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C101" s="41" t="s">
+      <c r="C102" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D101" s="42"/>
-      <c r="E101" s="43"/>
-      <c r="F101" s="40" t="s">
+      <c r="D102" s="42"/>
+      <c r="E102" s="43"/>
+      <c r="F102" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G101" s="40"/>
-      <c r="H101" s="40" t="s">
+      <c r="G102" s="40"/>
+      <c r="H102" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I101" s="44"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="36">
-        <f>A101+1</f>
-        <v>2</v>
-      </c>
-      <c r="B102" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="C102" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" s="37">
-        <v>50</v>
-      </c>
-      <c r="E102" s="38"/>
-      <c r="F102" s="36"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="68"/>
-      <c r="I102" s="36"/>
+      <c r="I102" s="44"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="36">
-        <f t="shared" ref="A103:A105" si="4">A102+1</f>
-        <v>3</v>
+        <f>A102+1</f>
+        <v>2</v>
       </c>
       <c r="B103" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C103" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D103" s="37">
-        <v>500</v>
-      </c>
-      <c r="E103" s="38" t="s">
-        <v>17</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E103" s="38"/>
       <c r="F103" s="36"/>
       <c r="G103" s="36"/>
-      <c r="H103" s="36"/>
+      <c r="H103" s="68"/>
       <c r="I103" s="36"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A104:A106" si="5">A103+1</f>
+        <v>3</v>
+      </c>
+      <c r="B104" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C104" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="37">
+        <v>500</v>
+      </c>
+      <c r="E104" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F104" s="36"/>
+      <c r="G104" s="36"/>
+      <c r="H104" s="36"/>
+      <c r="I104" s="36"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="36">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="B104" s="27" t="s">
+      <c r="B105" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C104" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D104" s="28" t="s">
+      <c r="C105" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E104" s="8"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
-      <c r="I104" s="24"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="69">
-        <f t="shared" si="4"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="69">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="B105" s="69" t="s">
+      <c r="B106" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="C105" s="70" t="s">
+      <c r="C106" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="D105" s="71"/>
-      <c r="E105" s="72"/>
-      <c r="F105" s="69"/>
-      <c r="G105" s="73"/>
-      <c r="H105" s="73" t="s">
+      <c r="D106" s="71"/>
+      <c r="E106" s="72"/>
+      <c r="F106" s="69"/>
+      <c r="G106" s="73"/>
+      <c r="H106" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="I105" s="69"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="74">
+      <c r="I106" s="69"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="74">
         <v>6</v>
       </c>
-      <c r="B106" s="74" t="s">
+      <c r="B107" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C106" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="75" t="s">
+      <c r="C107" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="74"/>
+      <c r="E107" s="74"/>
+      <c r="F107" s="74"/>
+      <c r="G107" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="H106" s="75" t="s">
+      <c r="H107" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="I106" s="74"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="110" t="s">
+      <c r="I107" s="74"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="B110" s="111"/>
-      <c r="C110" s="111"/>
-      <c r="D110" s="111"/>
-      <c r="E110" s="111"/>
-      <c r="F110" s="77"/>
-      <c r="G110" s="77"/>
-      <c r="H110" s="77"/>
-      <c r="I110" s="77"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="78" t="s">
+      <c r="B111" s="124"/>
+      <c r="C111" s="124"/>
+      <c r="D111" s="124"/>
+      <c r="E111" s="124"/>
+      <c r="F111" s="77"/>
+      <c r="G111" s="77"/>
+      <c r="H111" s="77"/>
+      <c r="I111" s="77"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B111" s="78" t="s">
+      <c r="B112" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C111" s="78" t="s">
+      <c r="C112" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D111" s="78" t="s">
+      <c r="D112" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E111" s="78" t="s">
+      <c r="E112" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F111" s="78" t="s">
+      <c r="F112" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="G111" s="78" t="s">
+      <c r="G112" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="H111" s="78" t="s">
+      <c r="H112" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="I111" s="78" t="s">
+      <c r="I112" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="79">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" s="79">
         <v>1</v>
       </c>
-      <c r="B112" s="79" t="s">
+      <c r="B113" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C112" s="80" t="s">
+      <c r="C113" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D112" s="81">
+      <c r="D113" s="81">
         <v>50</v>
       </c>
-      <c r="E112" s="82"/>
-      <c r="F112" s="79" t="s">
+      <c r="E113" s="82"/>
+      <c r="F113" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G112" s="79"/>
-      <c r="H112" s="79"/>
-      <c r="I112" s="79"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="83">
-        <v>2</v>
-      </c>
-      <c r="B113" s="83" t="s">
-        <v>54</v>
-      </c>
-      <c r="C113" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D113" s="85">
-        <v>50</v>
-      </c>
-      <c r="E113" s="86"/>
-      <c r="F113" s="83"/>
-      <c r="G113" s="83"/>
-      <c r="H113" s="83"/>
-      <c r="I113" s="83"/>
+      <c r="G113" s="79"/>
+      <c r="H113" s="79"/>
+      <c r="I113" s="79"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B114" s="83" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C114" s="84" t="s">
         <v>14</v>
@@ -3249,10 +3262,10 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B115" s="83" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C115" s="84" t="s">
         <v>14</v>
@@ -3260,9 +3273,7 @@
       <c r="D115" s="85">
         <v>50</v>
       </c>
-      <c r="E115" s="86" t="s">
-        <v>17</v>
-      </c>
+      <c r="E115" s="86"/>
       <c r="F115" s="83"/>
       <c r="G115" s="83"/>
       <c r="H115" s="83"/>
@@ -3270,75 +3281,85 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B116" s="83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C116" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D116" s="85">
-        <v>500</v>
-      </c>
-      <c r="E116" s="86"/>
+        <v>50</v>
+      </c>
+      <c r="E116" s="86" t="s">
+        <v>17</v>
+      </c>
       <c r="F116" s="83"/>
       <c r="G116" s="83"/>
-      <c r="H116" s="68" t="s">
-        <v>68</v>
-      </c>
+      <c r="H116" s="83"/>
       <c r="I116" s="83"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B117" s="83" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C117" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D117" s="85">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E117" s="86"/>
       <c r="F117" s="83"/>
       <c r="G117" s="83"/>
-      <c r="H117" s="83" t="s">
+      <c r="H117" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="I117" s="83"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" s="83">
+        <v>6</v>
+      </c>
+      <c r="B118" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D118" s="85">
+        <v>50</v>
+      </c>
+      <c r="E118" s="86"/>
+      <c r="F118" s="83"/>
+      <c r="G118" s="83"/>
+      <c r="H118" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="I117" s="83"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="98">
+      <c r="I118" s="83"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" s="98">
         <v>7</v>
       </c>
-      <c r="B118" s="98" t="s">
+      <c r="B119" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="C118" s="99" t="s">
+      <c r="C119" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="D118" s="100"/>
-      <c r="E118" s="101" t="s">
+      <c r="D119" s="100"/>
+      <c r="E119" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F118" s="98"/>
-      <c r="G118" s="98"/>
-      <c r="H118" s="98"/>
-      <c r="I118" s="98"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="94"/>
-      <c r="B119" s="94"/>
-      <c r="C119" s="95"/>
-      <c r="D119" s="96"/>
-      <c r="E119" s="97"/>
-      <c r="F119" s="94"/>
-      <c r="G119" s="94"/>
-      <c r="H119" s="94"/>
-      <c r="I119" s="94"/>
+      <c r="F119" s="98"/>
+      <c r="G119" s="98"/>
+      <c r="H119" s="98"/>
+      <c r="I119" s="98"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="94"/>
@@ -3352,125 +3373,115 @@
       <c r="I120" s="94"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="102"/>
-      <c r="B121" s="102"/>
-      <c r="C121" s="102"/>
-      <c r="D121" s="102"/>
-      <c r="E121" s="102"/>
-      <c r="F121" s="102"/>
-      <c r="G121" s="102"/>
-      <c r="H121" s="102"/>
-      <c r="I121" s="102"/>
+      <c r="A121" s="94"/>
+      <c r="B121" s="94"/>
+      <c r="C121" s="95"/>
+      <c r="D121" s="96"/>
+      <c r="E121" s="97"/>
+      <c r="F121" s="94"/>
+      <c r="G121" s="94"/>
+      <c r="H121" s="94"/>
+      <c r="I121" s="94"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="112" t="s">
+      <c r="A122" s="102"/>
+      <c r="B122" s="102"/>
+      <c r="C122" s="102"/>
+      <c r="D122" s="102"/>
+      <c r="E122" s="102"/>
+      <c r="F122" s="102"/>
+      <c r="G122" s="102"/>
+      <c r="H122" s="102"/>
+      <c r="I122" s="102"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="B122" s="111"/>
-      <c r="C122" s="111"/>
-      <c r="D122" s="111"/>
-      <c r="E122" s="111"/>
-      <c r="F122" s="87"/>
-      <c r="G122" s="87"/>
-      <c r="H122" s="87"/>
-      <c r="I122" s="87"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="88" t="s">
+      <c r="B123" s="124"/>
+      <c r="C123" s="124"/>
+      <c r="D123" s="124"/>
+      <c r="E123" s="124"/>
+      <c r="F123" s="87"/>
+      <c r="G123" s="87"/>
+      <c r="H123" s="87"/>
+      <c r="I123" s="87"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B123" s="88" t="s">
+      <c r="B124" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C123" s="88" t="s">
+      <c r="C124" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D123" s="88" t="s">
+      <c r="D124" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E123" s="88" t="s">
+      <c r="E124" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F123" s="88" t="s">
+      <c r="F124" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G123" s="88" t="s">
+      <c r="G124" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H123" s="88" t="s">
+      <c r="H124" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I123" s="88" t="s">
+      <c r="I124" s="88" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="1">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
         <v>1</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C124" s="89" t="s">
+      <c r="C125" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D124" s="90"/>
-      <c r="E124" s="91"/>
-      <c r="F124" s="1" t="s">
+      <c r="D125" s="90"/>
+      <c r="E125" s="91"/>
+      <c r="F125" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1" t="s">
+      <c r="G125" s="1"/>
+      <c r="H125" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I124" s="1"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="2">
-        <v>2</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D125" s="92">
-        <v>50</v>
-      </c>
-      <c r="E125" s="93"/>
-      <c r="F125" s="6"/>
-      <c r="G125" s="6"/>
-      <c r="H125" s="6"/>
-      <c r="I125" s="6"/>
+      <c r="I125" s="1"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D126" s="4"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="2">
-        <v>0</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I126" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D126" s="92">
+        <v>50</v>
+      </c>
+      <c r="E126" s="93"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>42</v>
@@ -3482,16 +3493,16 @@
         <v>0</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>42</v>
@@ -3502,36 +3513,36 @@
       <c r="G128" s="2">
         <v>0</v>
       </c>
-      <c r="H128" s="2"/>
+      <c r="H128" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="I128" s="2"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="5"/>
-      <c r="F129" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G129" s="2"/>
-      <c r="H129" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2">
+        <v>0</v>
+      </c>
+      <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>10</v>
@@ -3543,159 +3554,174 @@
       </c>
       <c r="G130" s="2"/>
       <c r="H130" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I130" s="2"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
+        <v>7</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131" s="4"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G131" s="2"/>
+      <c r="H131" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I131" s="2"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
         <v>8</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C131" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D131" s="4" t="s">
+      <c r="C132" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E131" s="5"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="2"/>
-      <c r="H131" s="6"/>
-      <c r="I131" s="2"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A132" s="103">
-        <v>9</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D132" s="4"/>
       <c r="E132" s="5"/>
       <c r="F132" s="6"/>
       <c r="G132" s="2"/>
       <c r="H132" s="6"/>
-      <c r="I132" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="I132" s="2"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="103">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="5"/>
       <c r="F133" s="6"/>
       <c r="G133" s="2"/>
       <c r="H133" s="6"/>
-      <c r="I133" s="2"/>
+      <c r="I133" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" s="2">
-        <v>11</v>
+      <c r="A134" s="103">
+        <v>10</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C134" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="5"/>
       <c r="F134" s="6"/>
       <c r="G134" s="2"/>
       <c r="H134" s="6"/>
-      <c r="I134" s="2" t="s">
+      <c r="I134" s="2"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>11</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D135" s="4"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="6"/>
+      <c r="I135" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A135" s="7">
-        <v>12</v>
-      </c>
-      <c r="B135" s="7" t="s">
+    <row r="136" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B136" s="128"/>
+      <c r="C136" s="93"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B137" s="17"/>
+      <c r="C137" s="129"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C138" s="111"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C139" s="111"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B141" s="110" t="s">
         <v>134</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C136" s="127"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C137" s="127"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C138" s="127"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B140" s="126" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B142" s="7" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B143" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B144" s="7" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B145" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="7" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B147" s="7" t="s">
+      <c r="B148" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B150" s="7" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B151" s="7" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="A123:E123"/>
+    <mergeCell ref="A43:A53"/>
+    <mergeCell ref="A73:I74"/>
+    <mergeCell ref="E56:I56"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A67:A70"/>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A12:I13"/>
     <mergeCell ref="A24:I25"/>
-    <mergeCell ref="A85:I86"/>
-    <mergeCell ref="A98:I99"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="A110:E110"/>
-    <mergeCell ref="A122:E122"/>
-    <mergeCell ref="A42:A52"/>
-    <mergeCell ref="A72:I73"/>
-    <mergeCell ref="E55:I55"/>
-    <mergeCell ref="A60:A65"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A86:I87"/>
+    <mergeCell ref="A99:I100"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="A33:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>